<commit_message>
Solved some question in final 450
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\B.TeCh\Competative Programming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Practice\Final 450\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="468">
   <si>
     <t>Questions by Love Babbar:</t>
   </si>
@@ -1431,6 +1431,9 @@
   </si>
   <si>
     <t xml:space="preserve">yes </t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -1862,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2770,7 +2773,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="21">
@@ -2907,7 +2910,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -2918,7 +2921,7 @@
         <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2940,7 +2943,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -4352,7 +4355,7 @@
         <v>231</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
@@ -4363,7 +4366,7 @@
         <v>232</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="21">
@@ -4396,7 +4399,7 @@
         <v>235</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved some more questions
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Coding Practice\Final 450\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1110"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1439,7 +1434,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -1609,7 +1604,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1661,7 +1656,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1855,18 +1850,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A399" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C419" sqref="C419"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1985,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -2040,7 +2035,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2216,7 +2211,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2317,7 +2312,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2328,7 +2323,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2339,7 +2334,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">
@@ -2361,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some more question
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C108" sqref="C108"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C358" sqref="C358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2998,7 +2998,7 @@
         <v>106</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="21">
@@ -3009,7 +3009,7 @@
         <v>107</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21">
@@ -5608,7 +5608,7 @@
         <v>345</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5619,7 +5619,7 @@
         <v>346</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">

</xml_diff>

<commit_message>
almost done with array
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2155,7 +2155,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2166,7 +2166,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2177,7 +2177,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2188,7 +2188,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2243,7 +2243,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2254,7 +2254,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2265,7 +2265,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2276,7 +2276,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Done with manipulating bits
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A472" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C481" sqref="C481"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6899,7 +6899,7 @@
         <v>460</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="479" spans="1:3" ht="21">
@@ -6910,7 +6910,7 @@
         <v>461</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="480" spans="1:3" ht="21">
@@ -6921,7 +6921,7 @@
         <v>462</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="481" spans="1:3" ht="21">
@@ -6932,7 +6932,7 @@
         <v>463</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started solving tree problems
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A472" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C481" sqref="C481"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3711,7 +3711,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3722,7 +3722,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3733,7 +3733,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3744,7 +3744,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3755,7 +3755,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some questions in BT
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3766,7 +3766,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3777,7 +3777,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3788,7 +3788,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3799,7 +3799,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3810,7 +3810,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3821,7 +3821,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3832,7 +3832,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3843,7 +3843,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">
@@ -3854,7 +3854,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3865,7 +3865,7 @@
         <v>186</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -4106,7 +4106,7 @@
         <v>208</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Almost done with greedy
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C191" sqref="C191"/>
+    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4128,7 +4128,7 @@
         <v>210</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4150,7 +4150,7 @@
         <v>212</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4411,7 +4411,7 @@
         <v>236</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="21">
@@ -4422,7 +4422,7 @@
         <v>237</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>4</v>
+        <v>467</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="21">
@@ -4433,7 +4433,7 @@
         <v>238</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="21">
@@ -4444,7 +4444,7 @@
         <v>239</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="21">
@@ -4455,7 +4455,7 @@
         <v>240</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="21">
@@ -4488,7 +4488,7 @@
         <v>243</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="21">
@@ -4499,7 +4499,7 @@
         <v>244</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="21">
@@ -4510,7 +4510,7 @@
         <v>245</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="21">
@@ -4521,7 +4521,7 @@
         <v>246</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="21">
@@ -4543,7 +4543,7 @@
         <v>248</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="21">
@@ -4554,7 +4554,7 @@
         <v>249</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="21">
@@ -4565,7 +4565,7 @@
         <v>250</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="21">
@@ -4598,7 +4598,7 @@
         <v>253</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="21">
@@ -4697,7 +4697,7 @@
         <v>262</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved some trie problems
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A233" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B265" sqref="B265"/>
+    <sheetView tabSelected="1" topLeftCell="A394" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C403" sqref="C403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4389,7 +4389,7 @@
         <v>234</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="21">
@@ -6090,7 +6090,7 @@
         <v>388</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="21">
@@ -6101,7 +6101,7 @@
         <v>389</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">

</xml_diff>

<commit_message>
completed all questions of Trie
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1199,9 +1199,6 @@
     <t>Word Break Problem | (Trie solution)</t>
   </si>
   <si>
-    <t>Implement a Phone Directory</t>
-  </si>
-  <si>
     <t>Print unique rows in a given boolean matrix</t>
   </si>
   <si>
@@ -1428,6 +1425,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Implement a Phone Directory[V.I.P]</t>
   </si>
 </sst>
 </file>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C403" sqref="C403"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21">
@@ -1913,7 +1913,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="21">
@@ -1924,7 +1924,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="21">
@@ -1935,7 +1935,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21">
@@ -1946,7 +1946,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="21">
@@ -1957,7 +1957,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="21">
@@ -1968,7 +1968,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">
@@ -1979,7 +1979,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -1990,7 +1990,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">
@@ -2001,7 +2001,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="21">
@@ -2012,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21">
@@ -2023,7 +2023,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21">
@@ -2034,7 +2034,7 @@
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21">
@@ -2045,7 +2045,7 @@
         <v>18</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21">
@@ -2056,7 +2056,7 @@
         <v>19</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21">
@@ -2067,7 +2067,7 @@
         <v>20</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21">
@@ -2078,7 +2078,7 @@
         <v>21</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="21">
@@ -2089,7 +2089,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21">
@@ -2100,7 +2100,7 @@
         <v>23</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="21">
@@ -2111,7 +2111,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21">
@@ -2122,7 +2122,7 @@
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21">
@@ -2133,7 +2133,7 @@
         <v>26</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21">
@@ -2144,7 +2144,7 @@
         <v>27</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="21">
@@ -2155,7 +2155,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="21">
@@ -2166,7 +2166,7 @@
         <v>29</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="21">
@@ -2177,7 +2177,7 @@
         <v>30</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="21">
@@ -2188,7 +2188,7 @@
         <v>31</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21">
@@ -2199,7 +2199,7 @@
         <v>32</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="21">
@@ -2210,7 +2210,7 @@
         <v>33</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="21">
@@ -2221,7 +2221,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="21">
@@ -2232,7 +2232,7 @@
         <v>35</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="21">
@@ -2243,7 +2243,7 @@
         <v>36</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="21">
@@ -2254,7 +2254,7 @@
         <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="21">
@@ -2265,7 +2265,7 @@
         <v>38</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="21">
@@ -2276,7 +2276,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="21">
@@ -2287,7 +2287,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="21">
@@ -2298,7 +2298,7 @@
         <v>41</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="21">
@@ -2318,7 +2318,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="21">
@@ -2329,7 +2329,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="21">
@@ -2340,7 +2340,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="21">
@@ -2351,7 +2351,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="21">
@@ -2362,7 +2362,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="21">
@@ -2373,7 +2373,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="21">
@@ -2384,7 +2384,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="21">
@@ -2395,7 +2395,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="21">
@@ -2406,7 +2406,7 @@
         <v>51</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="21">
@@ -2417,7 +2417,7 @@
         <v>52</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="21">
@@ -2433,7 +2433,7 @@
         <v>54</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="21">
@@ -2444,7 +2444,7 @@
         <v>55</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="21">
@@ -2455,7 +2455,7 @@
         <v>56</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="21">
@@ -2477,7 +2477,7 @@
         <v>58</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="21">
@@ -2488,7 +2488,7 @@
         <v>59</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="21">
@@ -2499,7 +2499,7 @@
         <v>60</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="21">
@@ -2510,7 +2510,7 @@
         <v>61</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="21">
@@ -2532,7 +2532,7 @@
         <v>63</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="21">
@@ -2587,7 +2587,7 @@
         <v>68</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="21">
@@ -2653,7 +2653,7 @@
         <v>74</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="21">
@@ -2752,7 +2752,7 @@
         <v>83</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="21">
@@ -2774,7 +2774,7 @@
         <v>85</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="21">
@@ -2884,7 +2884,7 @@
         <v>95</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="21">
@@ -2911,7 +2911,7 @@
         <v>98</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="21">
@@ -2922,7 +2922,7 @@
         <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="21">
@@ -2933,7 +2933,7 @@
         <v>100</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="21">
@@ -2944,7 +2944,7 @@
         <v>101</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="21">
@@ -2955,7 +2955,7 @@
         <v>102</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="21">
@@ -2977,7 +2977,7 @@
         <v>104</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="21">
@@ -2988,7 +2988,7 @@
         <v>105</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="21">
@@ -2999,7 +2999,7 @@
         <v>106</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="21">
@@ -3010,7 +3010,7 @@
         <v>107</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="21">
@@ -3021,7 +3021,7 @@
         <v>108</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="21">
@@ -3032,7 +3032,7 @@
         <v>109</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="21">
@@ -3043,7 +3043,7 @@
         <v>110</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="21">
@@ -3054,7 +3054,7 @@
         <v>111</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="21">
@@ -3065,7 +3065,7 @@
         <v>112</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="21">
@@ -3076,7 +3076,7 @@
         <v>113</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="21">
@@ -3087,7 +3087,7 @@
         <v>114</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="21">
@@ -3098,7 +3098,7 @@
         <v>115</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="21">
@@ -3109,7 +3109,7 @@
         <v>116</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="21">
@@ -3131,7 +3131,7 @@
         <v>118</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="21">
@@ -3142,7 +3142,7 @@
         <v>119</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="21">
@@ -3153,7 +3153,7 @@
         <v>120</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="21">
@@ -3164,7 +3164,7 @@
         <v>121</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="21">
@@ -3175,7 +3175,7 @@
         <v>122</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="21">
@@ -3186,7 +3186,7 @@
         <v>123</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="21">
@@ -3197,7 +3197,7 @@
         <v>124</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="21">
@@ -3208,7 +3208,7 @@
         <v>125</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="21">
@@ -3219,7 +3219,7 @@
         <v>126</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="21">
@@ -3263,7 +3263,7 @@
         <v>130</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="21">
@@ -3311,7 +3311,7 @@
         <v>135</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="21">
@@ -3711,7 +3711,7 @@
         <v>172</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="21">
@@ -3722,7 +3722,7 @@
         <v>173</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="21">
@@ -3733,7 +3733,7 @@
         <v>174</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="21">
@@ -3744,7 +3744,7 @@
         <v>175</v>
       </c>
       <c r="C180" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="21">
@@ -3755,7 +3755,7 @@
         <v>176</v>
       </c>
       <c r="C181" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="182" spans="1:3" ht="21">
@@ -3766,7 +3766,7 @@
         <v>177</v>
       </c>
       <c r="C182" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="183" spans="1:3" ht="21">
@@ -3777,7 +3777,7 @@
         <v>178</v>
       </c>
       <c r="C183" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="184" spans="1:3" ht="21">
@@ -3788,7 +3788,7 @@
         <v>179</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="185" spans="1:3" ht="21">
@@ -3799,7 +3799,7 @@
         <v>180</v>
       </c>
       <c r="C185" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="186" spans="1:3" ht="21">
@@ -3810,7 +3810,7 @@
         <v>181</v>
       </c>
       <c r="C186" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="187" spans="1:3" ht="21">
@@ -3821,7 +3821,7 @@
         <v>182</v>
       </c>
       <c r="C187" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="188" spans="1:3" ht="21">
@@ -3832,7 +3832,7 @@
         <v>183</v>
       </c>
       <c r="C188" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="189" spans="1:3" ht="21">
@@ -3843,7 +3843,7 @@
         <v>184</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="190" spans="1:3" ht="21">
@@ -3854,7 +3854,7 @@
         <v>185</v>
       </c>
       <c r="C190" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="191" spans="1:3" ht="21">
@@ -3865,7 +3865,7 @@
         <v>186</v>
       </c>
       <c r="C191" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="192" spans="1:3" ht="21">
@@ -4106,7 +4106,7 @@
         <v>208</v>
       </c>
       <c r="C214" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="215" spans="1:3" ht="21">
@@ -4128,7 +4128,7 @@
         <v>210</v>
       </c>
       <c r="C216" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="217" spans="1:3" ht="21">
@@ -4150,7 +4150,7 @@
         <v>212</v>
       </c>
       <c r="C218" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="219" spans="1:3" ht="21">
@@ -4356,7 +4356,7 @@
         <v>231</v>
       </c>
       <c r="C238" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="239" spans="1:3" ht="21">
@@ -4367,7 +4367,7 @@
         <v>232</v>
       </c>
       <c r="C239" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="240" spans="1:3" ht="21">
@@ -4389,7 +4389,7 @@
         <v>234</v>
       </c>
       <c r="C241" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="242" spans="1:3" ht="21">
@@ -4400,7 +4400,7 @@
         <v>235</v>
       </c>
       <c r="C242" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="243" spans="1:3" ht="21">
@@ -4411,7 +4411,7 @@
         <v>236</v>
       </c>
       <c r="C243" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="244" spans="1:3" ht="21">
@@ -4422,7 +4422,7 @@
         <v>237</v>
       </c>
       <c r="C244" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="245" spans="1:3" ht="21">
@@ -4433,7 +4433,7 @@
         <v>238</v>
       </c>
       <c r="C245" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="21">
@@ -4444,7 +4444,7 @@
         <v>239</v>
       </c>
       <c r="C246" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="21">
@@ -4455,7 +4455,7 @@
         <v>240</v>
       </c>
       <c r="C247" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="21">
@@ -4488,7 +4488,7 @@
         <v>243</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="21">
@@ -4499,7 +4499,7 @@
         <v>244</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="252" spans="1:3" ht="21">
@@ -4510,7 +4510,7 @@
         <v>245</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="21">
@@ -4521,7 +4521,7 @@
         <v>246</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="254" spans="1:3" ht="21">
@@ -4532,7 +4532,7 @@
         <v>247</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="255" spans="1:3" ht="21">
@@ -4543,7 +4543,7 @@
         <v>248</v>
       </c>
       <c r="C255" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="256" spans="1:3" ht="21">
@@ -4554,7 +4554,7 @@
         <v>249</v>
       </c>
       <c r="C256" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="257" spans="1:3" ht="21">
@@ -4565,7 +4565,7 @@
         <v>250</v>
       </c>
       <c r="C257" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="21">
@@ -4598,7 +4598,7 @@
         <v>253</v>
       </c>
       <c r="C260" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="261" spans="1:3" ht="21">
@@ -4609,7 +4609,7 @@
         <v>254</v>
       </c>
       <c r="C261" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="21">
@@ -4697,7 +4697,7 @@
         <v>262</v>
       </c>
       <c r="C269" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="270" spans="1:3" ht="21">
@@ -4708,7 +4708,7 @@
         <v>263</v>
       </c>
       <c r="C270" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="271" spans="1:3" ht="21">
@@ -4966,7 +4966,7 @@
         <v>286</v>
       </c>
       <c r="C296" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="21">
@@ -4977,7 +4977,7 @@
         <v>287</v>
       </c>
       <c r="C297" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="298" spans="1:3" ht="21">
@@ -4988,7 +4988,7 @@
         <v>288</v>
       </c>
       <c r="C298" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="299" spans="1:3" ht="21">
@@ -5021,7 +5021,7 @@
         <v>291</v>
       </c>
       <c r="C301" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="302" spans="1:3" ht="21">
@@ -5032,7 +5032,7 @@
         <v>292</v>
       </c>
       <c r="C302" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="303" spans="1:3" ht="21">
@@ -5043,7 +5043,7 @@
         <v>293</v>
       </c>
       <c r="C303" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="304" spans="1:3" ht="21">
@@ -5054,7 +5054,7 @@
         <v>294</v>
       </c>
       <c r="C304" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="305" spans="1:3" ht="21">
@@ -5065,7 +5065,7 @@
         <v>295</v>
       </c>
       <c r="C305" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="306" spans="1:3" ht="21">
@@ -5076,7 +5076,7 @@
         <v>296</v>
       </c>
       <c r="C306" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="307" spans="1:3" ht="21">
@@ -5087,7 +5087,7 @@
         <v>297</v>
       </c>
       <c r="C307" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="308" spans="1:3" ht="21">
@@ -5109,7 +5109,7 @@
         <v>299</v>
       </c>
       <c r="C309" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="310" spans="1:3" ht="21">
@@ -5120,7 +5120,7 @@
         <v>300</v>
       </c>
       <c r="C310" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="311" spans="1:3" ht="21">
@@ -5131,7 +5131,7 @@
         <v>301</v>
       </c>
       <c r="C311" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="312" spans="1:3" ht="21">
@@ -5373,7 +5373,7 @@
         <v>323</v>
       </c>
       <c r="C333" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="334" spans="1:3" ht="21">
@@ -5609,7 +5609,7 @@
         <v>345</v>
       </c>
       <c r="C357" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="21">
@@ -5620,7 +5620,7 @@
         <v>346</v>
       </c>
       <c r="C358" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="359" spans="1:3" ht="21">
@@ -5818,7 +5818,7 @@
         <v>364</v>
       </c>
       <c r="C376" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="377" spans="1:3" ht="21">
@@ -6090,7 +6090,7 @@
         <v>388</v>
       </c>
       <c r="C402" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="403" spans="1:3" ht="21">
@@ -6101,7 +6101,7 @@
         <v>389</v>
       </c>
       <c r="C403" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="404" spans="1:3" ht="21">
@@ -6112,7 +6112,7 @@
         <v>390</v>
       </c>
       <c r="C404" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="405" spans="1:3" ht="21">
@@ -6123,7 +6123,7 @@
         <v>89</v>
       </c>
       <c r="C405" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="406" spans="1:3" ht="21">
@@ -6131,10 +6131,10 @@
         <v>387</v>
       </c>
       <c r="B406" s="6" t="s">
-        <v>391</v>
+        <v>467</v>
       </c>
       <c r="C406" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="407" spans="1:3" ht="21">
@@ -6142,10 +6142,10 @@
         <v>387</v>
       </c>
       <c r="B407" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C407" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="408" spans="1:3" ht="21">
@@ -6158,32 +6158,32 @@
     </row>
     <row r="410" spans="1:3" ht="21">
       <c r="A410" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="B410" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="B410" s="6" t="s">
-        <v>394</v>
-      </c>
       <c r="C410" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="411" spans="1:3" ht="21">
       <c r="A411" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B411" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C411" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="412" spans="1:3" ht="21">
       <c r="A412" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B412" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C412" s="4" t="s">
         <v>4</v>
@@ -6191,10 +6191,10 @@
     </row>
     <row r="413" spans="1:3" ht="21">
       <c r="A413" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B413" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C413" s="4" t="s">
         <v>4</v>
@@ -6202,10 +6202,10 @@
     </row>
     <row r="414" spans="1:3" ht="21">
       <c r="A414" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B414" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C414" s="4" t="s">
         <v>4</v>
@@ -6213,10 +6213,10 @@
     </row>
     <row r="415" spans="1:3" ht="21">
       <c r="A415" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B415" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C415" s="4" t="s">
         <v>4</v>
@@ -6224,10 +6224,10 @@
     </row>
     <row r="416" spans="1:3" ht="21">
       <c r="A416" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B416" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C416" s="4" t="s">
         <v>4</v>
@@ -6235,7 +6235,7 @@
     </row>
     <row r="417" spans="1:3" ht="21">
       <c r="A417" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B417" s="6" t="s">
         <v>273</v>
@@ -6246,10 +6246,10 @@
     </row>
     <row r="418" spans="1:3" ht="21">
       <c r="A418" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B418" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C418" s="4" t="s">
         <v>4</v>
@@ -6257,21 +6257,21 @@
     </row>
     <row r="419" spans="1:3" ht="21">
       <c r="A419" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B419" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C419" s="4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="420" spans="1:3" ht="21">
       <c r="A420" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B420" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C420" s="4" t="s">
         <v>4</v>
@@ -6279,10 +6279,10 @@
     </row>
     <row r="421" spans="1:3" ht="21">
       <c r="A421" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B421" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C421" s="4" t="s">
         <v>4</v>
@@ -6290,10 +6290,10 @@
     </row>
     <row r="422" spans="1:3" ht="21">
       <c r="A422" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B422" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C422" s="4" t="s">
         <v>4</v>
@@ -6301,10 +6301,10 @@
     </row>
     <row r="423" spans="1:3" ht="21">
       <c r="A423" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B423" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C423" s="4" t="s">
         <v>4</v>
@@ -6312,10 +6312,10 @@
     </row>
     <row r="424" spans="1:3" ht="21">
       <c r="A424" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B424" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C424" s="4" t="s">
         <v>4</v>
@@ -6323,10 +6323,10 @@
     </row>
     <row r="425" spans="1:3" ht="21">
       <c r="A425" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B425" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C425" s="4" t="s">
         <v>4</v>
@@ -6334,10 +6334,10 @@
     </row>
     <row r="426" spans="1:3" ht="21">
       <c r="A426" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B426" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C426" s="4" t="s">
         <v>4</v>
@@ -6345,10 +6345,10 @@
     </row>
     <row r="427" spans="1:3" ht="21">
       <c r="A427" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B427" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C427" s="4" t="s">
         <v>4</v>
@@ -6356,10 +6356,10 @@
     </row>
     <row r="428" spans="1:3" ht="21">
       <c r="A428" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B428" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C428" s="4" t="s">
         <v>4</v>
@@ -6367,10 +6367,10 @@
     </row>
     <row r="429" spans="1:3" ht="21">
       <c r="A429" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B429" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C429" s="4" t="s">
         <v>4</v>
@@ -6378,10 +6378,10 @@
     </row>
     <row r="430" spans="1:3" ht="21">
       <c r="A430" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B430" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C430" s="4" t="s">
         <v>4</v>
@@ -6389,10 +6389,10 @@
     </row>
     <row r="431" spans="1:3" ht="21">
       <c r="A431" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B431" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C431" s="4" t="s">
         <v>4</v>
@@ -6400,21 +6400,21 @@
     </row>
     <row r="432" spans="1:3" ht="21">
       <c r="A432" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B432" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C432" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="433" spans="1:3" ht="21">
       <c r="A433" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B433" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C433" s="4" t="s">
         <v>4</v>
@@ -6422,10 +6422,10 @@
     </row>
     <row r="434" spans="1:3" ht="21">
       <c r="A434" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B434" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C434" s="4" t="s">
         <v>4</v>
@@ -6433,10 +6433,10 @@
     </row>
     <row r="435" spans="1:3" ht="21">
       <c r="A435" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B435" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C435" s="4" t="s">
         <v>4</v>
@@ -6444,10 +6444,10 @@
     </row>
     <row r="436" spans="1:3" ht="21">
       <c r="A436" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B436" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C436" s="4" t="s">
         <v>4</v>
@@ -6455,10 +6455,10 @@
     </row>
     <row r="437" spans="1:3" ht="21">
       <c r="A437" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B437" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C437" s="4" t="s">
         <v>4</v>
@@ -6466,10 +6466,10 @@
     </row>
     <row r="438" spans="1:3" ht="21">
       <c r="A438" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B438" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C438" s="4" t="s">
         <v>4</v>
@@ -6477,10 +6477,10 @@
     </row>
     <row r="439" spans="1:3" ht="21">
       <c r="A439" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B439" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C439" s="4" t="s">
         <v>4</v>
@@ -6488,10 +6488,10 @@
     </row>
     <row r="440" spans="1:3" ht="21">
       <c r="A440" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B440" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C440" s="4" t="s">
         <v>4</v>
@@ -6499,10 +6499,10 @@
     </row>
     <row r="441" spans="1:3" ht="21">
       <c r="A441" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B441" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C441" s="4" t="s">
         <v>4</v>
@@ -6510,10 +6510,10 @@
     </row>
     <row r="442" spans="1:3" ht="21">
       <c r="A442" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B442" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C442" s="4" t="s">
         <v>4</v>
@@ -6521,10 +6521,10 @@
     </row>
     <row r="443" spans="1:3" ht="21">
       <c r="A443" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B443" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C443" s="4" t="s">
         <v>4</v>
@@ -6532,21 +6532,21 @@
     </row>
     <row r="444" spans="1:3" ht="21">
       <c r="A444" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B444" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C444" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="445" spans="1:3" ht="21">
       <c r="A445" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B445" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C445" s="4" t="s">
         <v>4</v>
@@ -6554,10 +6554,10 @@
     </row>
     <row r="446" spans="1:3" ht="21">
       <c r="A446" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B446" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C446" s="4" t="s">
         <v>4</v>
@@ -6565,10 +6565,10 @@
     </row>
     <row r="447" spans="1:3" ht="21">
       <c r="A447" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B447" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C447" s="4" t="s">
         <v>4</v>
@@ -6576,10 +6576,10 @@
     </row>
     <row r="448" spans="1:3" ht="21">
       <c r="A448" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B448" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C448" s="4" t="s">
         <v>4</v>
@@ -6587,10 +6587,10 @@
     </row>
     <row r="449" spans="1:3" ht="21">
       <c r="A449" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B449" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C449" s="4" t="s">
         <v>4</v>
@@ -6598,10 +6598,10 @@
     </row>
     <row r="450" spans="1:3" ht="21">
       <c r="A450" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B450" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C450" s="4" t="s">
         <v>4</v>
@@ -6609,10 +6609,10 @@
     </row>
     <row r="451" spans="1:3" ht="21">
       <c r="A451" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B451" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C451" s="4" t="s">
         <v>4</v>
@@ -6620,21 +6620,21 @@
     </row>
     <row r="452" spans="1:3" ht="21">
       <c r="A452" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B452" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C452" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="453" spans="1:3" ht="21">
       <c r="A453" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B453" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C453" s="4" t="s">
         <v>4</v>
@@ -6642,10 +6642,10 @@
     </row>
     <row r="454" spans="1:3" ht="21">
       <c r="A454" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B454" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C454" s="4" t="s">
         <v>4</v>
@@ -6653,10 +6653,10 @@
     </row>
     <row r="455" spans="1:3" ht="21">
       <c r="A455" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B455" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C455" s="4" t="s">
         <v>4</v>
@@ -6664,10 +6664,10 @@
     </row>
     <row r="456" spans="1:3" ht="21">
       <c r="A456" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B456" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C456" s="4" t="s">
         <v>4</v>
@@ -6675,10 +6675,10 @@
     </row>
     <row r="457" spans="1:3" ht="21">
       <c r="A457" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B457" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C457" s="4" t="s">
         <v>4</v>
@@ -6686,10 +6686,10 @@
     </row>
     <row r="458" spans="1:3" ht="21">
       <c r="A458" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B458" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C458" s="4" t="s">
         <v>4</v>
@@ -6697,10 +6697,10 @@
     </row>
     <row r="459" spans="1:3" ht="21">
       <c r="A459" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B459" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C459" s="4" t="s">
         <v>4</v>
@@ -6708,10 +6708,10 @@
     </row>
     <row r="460" spans="1:3" ht="21">
       <c r="A460" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B460" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C460" s="4" t="s">
         <v>4</v>
@@ -6719,10 +6719,10 @@
     </row>
     <row r="461" spans="1:3" ht="21">
       <c r="A461" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B461" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C461" s="4" t="s">
         <v>4</v>
@@ -6730,10 +6730,10 @@
     </row>
     <row r="462" spans="1:3" ht="21">
       <c r="A462" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B462" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C462" s="4" t="s">
         <v>4</v>
@@ -6741,10 +6741,10 @@
     </row>
     <row r="463" spans="1:3" ht="21">
       <c r="A463" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B463" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C463" s="4" t="s">
         <v>4</v>
@@ -6752,10 +6752,10 @@
     </row>
     <row r="464" spans="1:3" ht="21">
       <c r="A464" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B464" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C464" s="4" t="s">
         <v>4</v>
@@ -6763,10 +6763,10 @@
     </row>
     <row r="465" spans="1:3" ht="21">
       <c r="A465" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B465" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C465" s="4" t="s">
         <v>4</v>
@@ -6774,10 +6774,10 @@
     </row>
     <row r="466" spans="1:3" ht="21">
       <c r="A466" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B466" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C466" s="4" t="s">
         <v>4</v>
@@ -6785,10 +6785,10 @@
     </row>
     <row r="467" spans="1:3" ht="21">
       <c r="A467" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B467" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C467" s="4" t="s">
         <v>4</v>
@@ -6796,10 +6796,10 @@
     </row>
     <row r="468" spans="1:3" ht="21">
       <c r="A468" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B468" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C468" s="4" t="s">
         <v>4</v>
@@ -6807,10 +6807,10 @@
     </row>
     <row r="469" spans="1:3" ht="21">
       <c r="A469" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B469" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C469" s="4" t="s">
         <v>4</v>
@@ -6827,112 +6827,112 @@
     </row>
     <row r="472" spans="1:3" ht="21">
       <c r="A472" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="B472" s="6" t="s">
         <v>453</v>
       </c>
-      <c r="B472" s="6" t="s">
-        <v>454</v>
-      </c>
       <c r="C472" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="473" spans="1:3" ht="21">
       <c r="A473" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B473" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C473" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="474" spans="1:3" ht="21">
       <c r="A474" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B474" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C474" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="475" spans="1:3" ht="21">
       <c r="A475" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B475" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C475" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="476" spans="1:3" ht="21">
       <c r="A476" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B476" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C476" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="477" spans="1:3" ht="21">
       <c r="A477" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B477" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C477" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="478" spans="1:3" ht="21">
       <c r="A478" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B478" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="479" spans="1:3" ht="21">
       <c r="A479" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B479" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C479" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="480" spans="1:3" ht="21">
       <c r="A480" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B480" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C480" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="481" spans="1:3" ht="21">
       <c r="A481" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B481" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C481" s="4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
   </sheetData>
@@ -7309,7 +7309,7 @@
     <hyperlink ref="B403" r:id="rId370"/>
     <hyperlink ref="B404" r:id="rId371"/>
     <hyperlink ref="B405" r:id="rId372"/>
-    <hyperlink ref="B406" r:id="rId373"/>
+    <hyperlink ref="B406" r:id="rId373" display="Implement a Phone Directory"/>
     <hyperlink ref="B407" r:id="rId374"/>
     <hyperlink ref="B410" r:id="rId375"/>
     <hyperlink ref="B411" r:id="rId376"/>

</xml_diff>

<commit_message>
solved some string problems
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2521,7 +2521,7 @@
         <v>62</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="21">
@@ -2543,7 +2543,7 @@
         <v>64</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="21">
@@ -2554,7 +2554,7 @@
         <v>65</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="21">
@@ -2763,7 +2763,7 @@
         <v>84</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="21">
@@ -6307,7 +6307,7 @@
         <v>405</v>
       </c>
       <c r="C423" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="424" spans="1:3" ht="21">
@@ -6351,7 +6351,7 @@
         <v>409</v>
       </c>
       <c r="C427" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="428" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added some new files
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1871,7 +1871,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2598,7 +2598,7 @@
         <v>69</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="21">
@@ -2609,7 +2609,7 @@
         <v>70</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="21">
@@ -2620,7 +2620,7 @@
         <v>71</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="21">
@@ -2631,7 +2631,7 @@
         <v>72</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="21">
@@ -6997,392 +6997,392 @@
     <hyperlink ref="B68" r:id="rId58"/>
     <hyperlink ref="B69" r:id="rId59"/>
     <hyperlink ref="B70" r:id="rId60"/>
-    <hyperlink ref="B71" r:id="rId61"/>
-    <hyperlink ref="B72" r:id="rId62"/>
-    <hyperlink ref="B73" r:id="rId63"/>
-    <hyperlink ref="B74" r:id="rId64"/>
-    <hyperlink ref="B75" r:id="rId65"/>
-    <hyperlink ref="B76" r:id="rId66"/>
-    <hyperlink ref="B77" r:id="rId67"/>
-    <hyperlink ref="B78" r:id="rId68"/>
-    <hyperlink ref="B79" r:id="rId69"/>
-    <hyperlink ref="B80" r:id="rId70"/>
-    <hyperlink ref="B81" r:id="rId71"/>
-    <hyperlink ref="B82" r:id="rId72"/>
-    <hyperlink ref="B83" r:id="rId73"/>
-    <hyperlink ref="B84" r:id="rId74"/>
-    <hyperlink ref="B85" r:id="rId75"/>
-    <hyperlink ref="B86" r:id="rId76"/>
-    <hyperlink ref="B87" r:id="rId77"/>
-    <hyperlink ref="B88" r:id="rId78"/>
-    <hyperlink ref="B89" r:id="rId79"/>
-    <hyperlink ref="B90" r:id="rId80"/>
-    <hyperlink ref="B91" r:id="rId81"/>
-    <hyperlink ref="B92" r:id="rId82"/>
-    <hyperlink ref="B93" r:id="rId83"/>
-    <hyperlink ref="B94" r:id="rId84"/>
-    <hyperlink ref="B95" r:id="rId85"/>
-    <hyperlink ref="B96" r:id="rId86"/>
-    <hyperlink ref="B97" r:id="rId87"/>
-    <hyperlink ref="B98" r:id="rId88"/>
-    <hyperlink ref="B101" r:id="rId89"/>
-    <hyperlink ref="B102" r:id="rId90"/>
-    <hyperlink ref="B103" r:id="rId91"/>
-    <hyperlink ref="B104" r:id="rId92"/>
-    <hyperlink ref="B106" r:id="rId93" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
-    <hyperlink ref="B107" r:id="rId94"/>
-    <hyperlink ref="B108" r:id="rId95"/>
-    <hyperlink ref="B109" r:id="rId96"/>
-    <hyperlink ref="B110" r:id="rId97"/>
-    <hyperlink ref="B111" r:id="rId98"/>
-    <hyperlink ref="B113" r:id="rId99"/>
-    <hyperlink ref="B114" r:id="rId100"/>
-    <hyperlink ref="B115" r:id="rId101"/>
-    <hyperlink ref="B116" r:id="rId102"/>
-    <hyperlink ref="B117" r:id="rId103"/>
-    <hyperlink ref="B118" r:id="rId104"/>
-    <hyperlink ref="B119" r:id="rId105"/>
-    <hyperlink ref="B120" r:id="rId106"/>
-    <hyperlink ref="B121" r:id="rId107"/>
-    <hyperlink ref="B122" r:id="rId108"/>
-    <hyperlink ref="B123" r:id="rId109"/>
-    <hyperlink ref="B124" r:id="rId110"/>
-    <hyperlink ref="B125" r:id="rId111"/>
-    <hyperlink ref="B126" r:id="rId112"/>
-    <hyperlink ref="B127" r:id="rId113"/>
-    <hyperlink ref="B128" r:id="rId114"/>
-    <hyperlink ref="B129" r:id="rId115"/>
-    <hyperlink ref="B130" r:id="rId116"/>
-    <hyperlink ref="B131" r:id="rId117"/>
-    <hyperlink ref="B132" r:id="rId118"/>
-    <hyperlink ref="B133" r:id="rId119"/>
-    <hyperlink ref="B134" r:id="rId120"/>
-    <hyperlink ref="B135" r:id="rId121"/>
-    <hyperlink ref="B136" r:id="rId122"/>
-    <hyperlink ref="B105" r:id="rId123"/>
-    <hyperlink ref="B112" r:id="rId124"/>
-    <hyperlink ref="B139" r:id="rId125"/>
-    <hyperlink ref="B140" r:id="rId126"/>
-    <hyperlink ref="B141" r:id="rId127"/>
-    <hyperlink ref="B142" r:id="rId128"/>
-    <hyperlink ref="B143" r:id="rId129"/>
-    <hyperlink ref="B144" r:id="rId130"/>
-    <hyperlink ref="B145" r:id="rId131"/>
-    <hyperlink ref="B146" r:id="rId132"/>
-    <hyperlink ref="B147" r:id="rId133"/>
-    <hyperlink ref="B148" r:id="rId134"/>
-    <hyperlink ref="B149" r:id="rId135"/>
-    <hyperlink ref="B150" r:id="rId136"/>
-    <hyperlink ref="B151" r:id="rId137"/>
-    <hyperlink ref="B152" r:id="rId138"/>
-    <hyperlink ref="B153" r:id="rId139"/>
-    <hyperlink ref="B154" r:id="rId140"/>
-    <hyperlink ref="B155" r:id="rId141"/>
-    <hyperlink ref="B156" r:id="rId142"/>
-    <hyperlink ref="B157" r:id="rId143"/>
-    <hyperlink ref="B158" r:id="rId144"/>
-    <hyperlink ref="B159" r:id="rId145"/>
-    <hyperlink ref="B160" r:id="rId146"/>
-    <hyperlink ref="B161" r:id="rId147"/>
-    <hyperlink ref="B162" r:id="rId148"/>
-    <hyperlink ref="B163" r:id="rId149"/>
-    <hyperlink ref="B166" r:id="rId150"/>
-    <hyperlink ref="B167" r:id="rId151"/>
-    <hyperlink ref="B168" r:id="rId152"/>
-    <hyperlink ref="B169" r:id="rId153"/>
-    <hyperlink ref="B170" r:id="rId154"/>
-    <hyperlink ref="B171" r:id="rId155"/>
-    <hyperlink ref="B172" r:id="rId156"/>
-    <hyperlink ref="B173" r:id="rId157"/>
-    <hyperlink ref="B174" r:id="rId158"/>
-    <hyperlink ref="B177" r:id="rId159"/>
-    <hyperlink ref="B178" r:id="rId160"/>
-    <hyperlink ref="B179" r:id="rId161"/>
-    <hyperlink ref="B180" r:id="rId162"/>
-    <hyperlink ref="B181" r:id="rId163"/>
-    <hyperlink ref="B182" r:id="rId164"/>
-    <hyperlink ref="B183" r:id="rId165"/>
-    <hyperlink ref="B184" r:id="rId166"/>
-    <hyperlink ref="B185" r:id="rId167"/>
-    <hyperlink ref="B186" r:id="rId168"/>
-    <hyperlink ref="B187" r:id="rId169"/>
-    <hyperlink ref="B188" r:id="rId170"/>
-    <hyperlink ref="B189" r:id="rId171"/>
-    <hyperlink ref="B190" r:id="rId172"/>
-    <hyperlink ref="B191" r:id="rId173"/>
-    <hyperlink ref="B192" r:id="rId174"/>
-    <hyperlink ref="B193" r:id="rId175"/>
-    <hyperlink ref="B194" r:id="rId176"/>
-    <hyperlink ref="B195" r:id="rId177"/>
-    <hyperlink ref="B196" r:id="rId178"/>
-    <hyperlink ref="B197" r:id="rId179" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B198" r:id="rId180"/>
-    <hyperlink ref="B199" r:id="rId181"/>
-    <hyperlink ref="B200" r:id="rId182"/>
-    <hyperlink ref="B201" r:id="rId183"/>
-    <hyperlink ref="B202" r:id="rId184"/>
-    <hyperlink ref="B203" r:id="rId185" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B204" r:id="rId186"/>
-    <hyperlink ref="B205" r:id="rId187"/>
-    <hyperlink ref="B206" r:id="rId188"/>
-    <hyperlink ref="B207" r:id="rId189"/>
-    <hyperlink ref="B208" r:id="rId190"/>
-    <hyperlink ref="B209" r:id="rId191"/>
-    <hyperlink ref="B210" r:id="rId192"/>
-    <hyperlink ref="B211" r:id="rId193"/>
-    <hyperlink ref="B214" r:id="rId194"/>
-    <hyperlink ref="B215" r:id="rId195"/>
-    <hyperlink ref="B216" r:id="rId196"/>
-    <hyperlink ref="B217" r:id="rId197"/>
-    <hyperlink ref="B218" r:id="rId198"/>
-    <hyperlink ref="B219" r:id="rId199"/>
-    <hyperlink ref="B220" r:id="rId200"/>
-    <hyperlink ref="B221" r:id="rId201"/>
-    <hyperlink ref="B222" r:id="rId202"/>
-    <hyperlink ref="B223" r:id="rId203"/>
-    <hyperlink ref="B224" r:id="rId204"/>
-    <hyperlink ref="B225" r:id="rId205"/>
-    <hyperlink ref="B226" r:id="rId206"/>
-    <hyperlink ref="B227" r:id="rId207"/>
-    <hyperlink ref="B228" r:id="rId208"/>
-    <hyperlink ref="B229" r:id="rId209"/>
-    <hyperlink ref="B230" r:id="rId210"/>
-    <hyperlink ref="B231" r:id="rId211"/>
-    <hyperlink ref="B232" r:id="rId212"/>
-    <hyperlink ref="B233" r:id="rId213"/>
-    <hyperlink ref="B234" r:id="rId214"/>
-    <hyperlink ref="B235" r:id="rId215"/>
-    <hyperlink ref="B238" r:id="rId216"/>
-    <hyperlink ref="B239" r:id="rId217"/>
-    <hyperlink ref="B240" r:id="rId218"/>
-    <hyperlink ref="B241" r:id="rId219"/>
-    <hyperlink ref="B242" r:id="rId220"/>
-    <hyperlink ref="B243" r:id="rId221"/>
-    <hyperlink ref="B244" r:id="rId222"/>
-    <hyperlink ref="B245" r:id="rId223"/>
-    <hyperlink ref="B246" r:id="rId224"/>
-    <hyperlink ref="B247" r:id="rId225"/>
-    <hyperlink ref="B248" r:id="rId226"/>
-    <hyperlink ref="B249" r:id="rId227"/>
-    <hyperlink ref="B250" r:id="rId228"/>
-    <hyperlink ref="B251" r:id="rId229"/>
-    <hyperlink ref="B252" r:id="rId230"/>
-    <hyperlink ref="B253" r:id="rId231"/>
-    <hyperlink ref="B254" r:id="rId232"/>
-    <hyperlink ref="B255" r:id="rId233"/>
-    <hyperlink ref="B256" r:id="rId234"/>
-    <hyperlink ref="B257" r:id="rId235" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId236"/>
-    <hyperlink ref="B259" r:id="rId237"/>
-    <hyperlink ref="B260" r:id="rId238"/>
-    <hyperlink ref="B261" r:id="rId239"/>
-    <hyperlink ref="B262" r:id="rId240"/>
-    <hyperlink ref="B263" r:id="rId241"/>
-    <hyperlink ref="B264" r:id="rId242"/>
-    <hyperlink ref="B265" r:id="rId243"/>
-    <hyperlink ref="B266" r:id="rId244"/>
-    <hyperlink ref="B267" r:id="rId245"/>
-    <hyperlink ref="B268" r:id="rId246"/>
-    <hyperlink ref="B269" r:id="rId247"/>
-    <hyperlink ref="B270" r:id="rId248"/>
-    <hyperlink ref="B271" r:id="rId249"/>
-    <hyperlink ref="B272" r:id="rId250"/>
-    <hyperlink ref="B275" r:id="rId251"/>
-    <hyperlink ref="B276" r:id="rId252"/>
-    <hyperlink ref="B277" r:id="rId253"/>
-    <hyperlink ref="B278" r:id="rId254"/>
-    <hyperlink ref="B279" r:id="rId255"/>
-    <hyperlink ref="B280" r:id="rId256"/>
-    <hyperlink ref="B281" r:id="rId257"/>
-    <hyperlink ref="B282" r:id="rId258"/>
-    <hyperlink ref="B283" r:id="rId259"/>
-    <hyperlink ref="B284" r:id="rId260"/>
-    <hyperlink ref="B285" r:id="rId261"/>
-    <hyperlink ref="B286" r:id="rId262"/>
-    <hyperlink ref="B287" r:id="rId263"/>
-    <hyperlink ref="B288" r:id="rId264"/>
-    <hyperlink ref="B289" r:id="rId265"/>
-    <hyperlink ref="B290" r:id="rId266"/>
-    <hyperlink ref="B291" r:id="rId267"/>
-    <hyperlink ref="B292" r:id="rId268"/>
-    <hyperlink ref="B293" r:id="rId269"/>
-    <hyperlink ref="B296" r:id="rId270"/>
-    <hyperlink ref="B297" r:id="rId271"/>
-    <hyperlink ref="B298" r:id="rId272"/>
-    <hyperlink ref="B299" r:id="rId273"/>
-    <hyperlink ref="B300" r:id="rId274"/>
-    <hyperlink ref="B301" r:id="rId275"/>
-    <hyperlink ref="B302" r:id="rId276"/>
-    <hyperlink ref="B303" r:id="rId277"/>
-    <hyperlink ref="B304" r:id="rId278"/>
-    <hyperlink ref="B305" r:id="rId279"/>
-    <hyperlink ref="B306" r:id="rId280" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId281"/>
-    <hyperlink ref="B308" r:id="rId282"/>
-    <hyperlink ref="B309" r:id="rId283"/>
-    <hyperlink ref="B310" r:id="rId284"/>
-    <hyperlink ref="B311" r:id="rId285"/>
-    <hyperlink ref="B312" r:id="rId286"/>
-    <hyperlink ref="B313" r:id="rId287"/>
-    <hyperlink ref="B314" r:id="rId288"/>
-    <hyperlink ref="B315" r:id="rId289"/>
-    <hyperlink ref="B316" r:id="rId290"/>
-    <hyperlink ref="B317" r:id="rId291"/>
-    <hyperlink ref="B318" r:id="rId292"/>
-    <hyperlink ref="B319" r:id="rId293"/>
-    <hyperlink ref="B320" r:id="rId294"/>
-    <hyperlink ref="B321" r:id="rId295"/>
-    <hyperlink ref="B322" r:id="rId296"/>
-    <hyperlink ref="B323" r:id="rId297"/>
-    <hyperlink ref="B324" r:id="rId298"/>
-    <hyperlink ref="B325" r:id="rId299"/>
-    <hyperlink ref="B326" r:id="rId300"/>
-    <hyperlink ref="B327" r:id="rId301"/>
-    <hyperlink ref="B328" r:id="rId302"/>
-    <hyperlink ref="B329" r:id="rId303"/>
-    <hyperlink ref="B330" r:id="rId304"/>
-    <hyperlink ref="B331" r:id="rId305"/>
-    <hyperlink ref="B332" r:id="rId306"/>
-    <hyperlink ref="B333" r:id="rId307"/>
-    <hyperlink ref="B336" r:id="rId308"/>
-    <hyperlink ref="B337" r:id="rId309"/>
-    <hyperlink ref="B338" r:id="rId310"/>
-    <hyperlink ref="B339" r:id="rId311"/>
-    <hyperlink ref="B340" r:id="rId312"/>
-    <hyperlink ref="B341" r:id="rId313"/>
-    <hyperlink ref="B342" r:id="rId314"/>
-    <hyperlink ref="B343" r:id="rId315"/>
-    <hyperlink ref="B344" r:id="rId316"/>
-    <hyperlink ref="B345" r:id="rId317"/>
-    <hyperlink ref="B346" r:id="rId318"/>
-    <hyperlink ref="B347" r:id="rId319"/>
-    <hyperlink ref="B348" r:id="rId320"/>
-    <hyperlink ref="B349" r:id="rId321"/>
-    <hyperlink ref="B350" r:id="rId322"/>
-    <hyperlink ref="B351" r:id="rId323"/>
-    <hyperlink ref="B352" r:id="rId324"/>
-    <hyperlink ref="B353" r:id="rId325"/>
-    <hyperlink ref="B357" r:id="rId326"/>
-    <hyperlink ref="B358" r:id="rId327"/>
-    <hyperlink ref="B359" r:id="rId328"/>
-    <hyperlink ref="B360" r:id="rId329"/>
-    <hyperlink ref="B361" r:id="rId330"/>
-    <hyperlink ref="B362" r:id="rId331"/>
-    <hyperlink ref="B363" r:id="rId332"/>
-    <hyperlink ref="B364" r:id="rId333"/>
-    <hyperlink ref="B365" r:id="rId334"/>
-    <hyperlink ref="B366" r:id="rId335"/>
-    <hyperlink ref="B367" r:id="rId336"/>
-    <hyperlink ref="B368" r:id="rId337"/>
-    <hyperlink ref="B369" r:id="rId338"/>
-    <hyperlink ref="B370" r:id="rId339"/>
-    <hyperlink ref="B371" r:id="rId340"/>
-    <hyperlink ref="B372" r:id="rId341"/>
-    <hyperlink ref="B373" r:id="rId342"/>
-    <hyperlink ref="B374" r:id="rId343"/>
-    <hyperlink ref="B375" r:id="rId344"/>
-    <hyperlink ref="B376" r:id="rId345"/>
-    <hyperlink ref="B377" r:id="rId346"/>
-    <hyperlink ref="B378" r:id="rId347"/>
-    <hyperlink ref="B379" r:id="rId348" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId349"/>
-    <hyperlink ref="B381" r:id="rId350"/>
-    <hyperlink ref="B382" r:id="rId351"/>
-    <hyperlink ref="B383" r:id="rId352"/>
-    <hyperlink ref="B384" r:id="rId353"/>
-    <hyperlink ref="B385" r:id="rId354"/>
-    <hyperlink ref="B386" r:id="rId355"/>
-    <hyperlink ref="B387" r:id="rId356"/>
-    <hyperlink ref="B388" r:id="rId357"/>
-    <hyperlink ref="B389" r:id="rId358"/>
-    <hyperlink ref="B390" r:id="rId359"/>
-    <hyperlink ref="B391" r:id="rId360"/>
-    <hyperlink ref="B392" r:id="rId361"/>
-    <hyperlink ref="B393" r:id="rId362"/>
-    <hyperlink ref="B394" r:id="rId363"/>
-    <hyperlink ref="B396" r:id="rId364"/>
-    <hyperlink ref="B395" r:id="rId365"/>
-    <hyperlink ref="B397" r:id="rId366"/>
-    <hyperlink ref="B398" r:id="rId367"/>
-    <hyperlink ref="B399" r:id="rId368"/>
-    <hyperlink ref="B402" r:id="rId369"/>
-    <hyperlink ref="B403" r:id="rId370"/>
-    <hyperlink ref="B404" r:id="rId371"/>
-    <hyperlink ref="B405" r:id="rId372"/>
-    <hyperlink ref="B406" r:id="rId373" display="Implement a Phone Directory"/>
-    <hyperlink ref="B407" r:id="rId374"/>
-    <hyperlink ref="B410" r:id="rId375"/>
-    <hyperlink ref="B411" r:id="rId376"/>
-    <hyperlink ref="B412" r:id="rId377"/>
-    <hyperlink ref="B413" r:id="rId378"/>
-    <hyperlink ref="B414" r:id="rId379"/>
-    <hyperlink ref="B415" r:id="rId380"/>
-    <hyperlink ref="B416" r:id="rId381"/>
-    <hyperlink ref="B417" r:id="rId382"/>
-    <hyperlink ref="B418" r:id="rId383"/>
-    <hyperlink ref="B419" r:id="rId384"/>
-    <hyperlink ref="B420" r:id="rId385"/>
-    <hyperlink ref="B421" r:id="rId386"/>
-    <hyperlink ref="B422" r:id="rId387"/>
-    <hyperlink ref="B423" r:id="rId388"/>
-    <hyperlink ref="B424" r:id="rId389"/>
-    <hyperlink ref="B425" r:id="rId390"/>
-    <hyperlink ref="B426" r:id="rId391"/>
-    <hyperlink ref="B427" r:id="rId392"/>
-    <hyperlink ref="B428" r:id="rId393"/>
-    <hyperlink ref="B429" r:id="rId394"/>
-    <hyperlink ref="B430" r:id="rId395"/>
-    <hyperlink ref="B431" r:id="rId396"/>
-    <hyperlink ref="B432" r:id="rId397"/>
-    <hyperlink ref="B433" r:id="rId398"/>
-    <hyperlink ref="B434" r:id="rId399"/>
-    <hyperlink ref="B435" r:id="rId400"/>
-    <hyperlink ref="B436" r:id="rId401"/>
-    <hyperlink ref="B437" r:id="rId402"/>
-    <hyperlink ref="B438" r:id="rId403"/>
-    <hyperlink ref="B439" r:id="rId404"/>
-    <hyperlink ref="B440" r:id="rId405"/>
-    <hyperlink ref="B441" r:id="rId406"/>
-    <hyperlink ref="B442" r:id="rId407"/>
-    <hyperlink ref="B443" r:id="rId408"/>
-    <hyperlink ref="B444" r:id="rId409"/>
-    <hyperlink ref="B445" r:id="rId410"/>
-    <hyperlink ref="B446" r:id="rId411"/>
-    <hyperlink ref="B447" r:id="rId412"/>
-    <hyperlink ref="B448" r:id="rId413"/>
-    <hyperlink ref="B449" r:id="rId414"/>
-    <hyperlink ref="B451" r:id="rId415"/>
-    <hyperlink ref="B450" r:id="rId416"/>
-    <hyperlink ref="B452" r:id="rId417"/>
-    <hyperlink ref="B453" r:id="rId418"/>
-    <hyperlink ref="B454" r:id="rId419"/>
-    <hyperlink ref="B455" r:id="rId420"/>
-    <hyperlink ref="B456" r:id="rId421"/>
-    <hyperlink ref="B457" r:id="rId422"/>
-    <hyperlink ref="B458" r:id="rId423"/>
-    <hyperlink ref="B459" r:id="rId424"/>
-    <hyperlink ref="B460" r:id="rId425"/>
-    <hyperlink ref="B461" r:id="rId426"/>
-    <hyperlink ref="B462" r:id="rId427"/>
-    <hyperlink ref="B469" r:id="rId428"/>
-    <hyperlink ref="B468" r:id="rId429"/>
-    <hyperlink ref="B467" r:id="rId430"/>
-    <hyperlink ref="B466" r:id="rId431"/>
-    <hyperlink ref="B465" r:id="rId432"/>
-    <hyperlink ref="B464" r:id="rId433"/>
-    <hyperlink ref="B463" r:id="rId434"/>
-    <hyperlink ref="B472" r:id="rId435"/>
-    <hyperlink ref="B473" r:id="rId436"/>
-    <hyperlink ref="B474" r:id="rId437"/>
-    <hyperlink ref="B475" r:id="rId438"/>
-    <hyperlink ref="B476" r:id="rId439"/>
-    <hyperlink ref="B477" r:id="rId440"/>
-    <hyperlink ref="B478" r:id="rId441"/>
-    <hyperlink ref="B481" r:id="rId442"/>
-    <hyperlink ref="B479" r:id="rId443"/>
-    <hyperlink ref="B480" r:id="rId444" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId445"/>
-    <hyperlink ref="B2" r:id="rId446"/>
+    <hyperlink ref="B72" r:id="rId61"/>
+    <hyperlink ref="B73" r:id="rId62"/>
+    <hyperlink ref="B74" r:id="rId63"/>
+    <hyperlink ref="B75" r:id="rId64"/>
+    <hyperlink ref="B76" r:id="rId65"/>
+    <hyperlink ref="B77" r:id="rId66"/>
+    <hyperlink ref="B78" r:id="rId67"/>
+    <hyperlink ref="B79" r:id="rId68"/>
+    <hyperlink ref="B80" r:id="rId69"/>
+    <hyperlink ref="B81" r:id="rId70"/>
+    <hyperlink ref="B82" r:id="rId71"/>
+    <hyperlink ref="B83" r:id="rId72"/>
+    <hyperlink ref="B84" r:id="rId73"/>
+    <hyperlink ref="B85" r:id="rId74"/>
+    <hyperlink ref="B86" r:id="rId75"/>
+    <hyperlink ref="B87" r:id="rId76"/>
+    <hyperlink ref="B88" r:id="rId77"/>
+    <hyperlink ref="B89" r:id="rId78"/>
+    <hyperlink ref="B90" r:id="rId79"/>
+    <hyperlink ref="B91" r:id="rId80"/>
+    <hyperlink ref="B92" r:id="rId81"/>
+    <hyperlink ref="B93" r:id="rId82"/>
+    <hyperlink ref="B94" r:id="rId83"/>
+    <hyperlink ref="B95" r:id="rId84"/>
+    <hyperlink ref="B96" r:id="rId85"/>
+    <hyperlink ref="B97" r:id="rId86"/>
+    <hyperlink ref="B98" r:id="rId87"/>
+    <hyperlink ref="B101" r:id="rId88"/>
+    <hyperlink ref="B102" r:id="rId89"/>
+    <hyperlink ref="B103" r:id="rId90"/>
+    <hyperlink ref="B104" r:id="rId91"/>
+    <hyperlink ref="B106" r:id="rId92" location=":~:text=We%20need%20to%20find%20a,set%20of%20points%20is%20minimum.&amp;text=In%20above%20figure%20optimum%20location,is%20minimum%20obtainable%20total%20distance."/>
+    <hyperlink ref="B107" r:id="rId93"/>
+    <hyperlink ref="B108" r:id="rId94"/>
+    <hyperlink ref="B109" r:id="rId95"/>
+    <hyperlink ref="B110" r:id="rId96"/>
+    <hyperlink ref="B111" r:id="rId97"/>
+    <hyperlink ref="B113" r:id="rId98"/>
+    <hyperlink ref="B114" r:id="rId99"/>
+    <hyperlink ref="B115" r:id="rId100"/>
+    <hyperlink ref="B116" r:id="rId101"/>
+    <hyperlink ref="B117" r:id="rId102"/>
+    <hyperlink ref="B118" r:id="rId103"/>
+    <hyperlink ref="B119" r:id="rId104"/>
+    <hyperlink ref="B120" r:id="rId105"/>
+    <hyperlink ref="B121" r:id="rId106"/>
+    <hyperlink ref="B122" r:id="rId107"/>
+    <hyperlink ref="B123" r:id="rId108"/>
+    <hyperlink ref="B124" r:id="rId109"/>
+    <hyperlink ref="B125" r:id="rId110"/>
+    <hyperlink ref="B126" r:id="rId111"/>
+    <hyperlink ref="B127" r:id="rId112"/>
+    <hyperlink ref="B128" r:id="rId113"/>
+    <hyperlink ref="B129" r:id="rId114"/>
+    <hyperlink ref="B130" r:id="rId115"/>
+    <hyperlink ref="B131" r:id="rId116"/>
+    <hyperlink ref="B132" r:id="rId117"/>
+    <hyperlink ref="B133" r:id="rId118"/>
+    <hyperlink ref="B134" r:id="rId119"/>
+    <hyperlink ref="B135" r:id="rId120"/>
+    <hyperlink ref="B136" r:id="rId121"/>
+    <hyperlink ref="B105" r:id="rId122"/>
+    <hyperlink ref="B112" r:id="rId123"/>
+    <hyperlink ref="B139" r:id="rId124"/>
+    <hyperlink ref="B140" r:id="rId125"/>
+    <hyperlink ref="B141" r:id="rId126"/>
+    <hyperlink ref="B142" r:id="rId127"/>
+    <hyperlink ref="B143" r:id="rId128"/>
+    <hyperlink ref="B144" r:id="rId129"/>
+    <hyperlink ref="B145" r:id="rId130"/>
+    <hyperlink ref="B146" r:id="rId131"/>
+    <hyperlink ref="B147" r:id="rId132"/>
+    <hyperlink ref="B148" r:id="rId133"/>
+    <hyperlink ref="B149" r:id="rId134"/>
+    <hyperlink ref="B150" r:id="rId135"/>
+    <hyperlink ref="B151" r:id="rId136"/>
+    <hyperlink ref="B152" r:id="rId137"/>
+    <hyperlink ref="B153" r:id="rId138"/>
+    <hyperlink ref="B154" r:id="rId139"/>
+    <hyperlink ref="B155" r:id="rId140"/>
+    <hyperlink ref="B156" r:id="rId141"/>
+    <hyperlink ref="B157" r:id="rId142"/>
+    <hyperlink ref="B158" r:id="rId143"/>
+    <hyperlink ref="B159" r:id="rId144"/>
+    <hyperlink ref="B160" r:id="rId145"/>
+    <hyperlink ref="B161" r:id="rId146"/>
+    <hyperlink ref="B162" r:id="rId147"/>
+    <hyperlink ref="B163" r:id="rId148"/>
+    <hyperlink ref="B166" r:id="rId149"/>
+    <hyperlink ref="B167" r:id="rId150"/>
+    <hyperlink ref="B168" r:id="rId151"/>
+    <hyperlink ref="B169" r:id="rId152"/>
+    <hyperlink ref="B170" r:id="rId153"/>
+    <hyperlink ref="B171" r:id="rId154"/>
+    <hyperlink ref="B172" r:id="rId155"/>
+    <hyperlink ref="B173" r:id="rId156"/>
+    <hyperlink ref="B174" r:id="rId157"/>
+    <hyperlink ref="B177" r:id="rId158"/>
+    <hyperlink ref="B178" r:id="rId159"/>
+    <hyperlink ref="B179" r:id="rId160"/>
+    <hyperlink ref="B180" r:id="rId161"/>
+    <hyperlink ref="B181" r:id="rId162"/>
+    <hyperlink ref="B182" r:id="rId163"/>
+    <hyperlink ref="B183" r:id="rId164"/>
+    <hyperlink ref="B184" r:id="rId165"/>
+    <hyperlink ref="B185" r:id="rId166"/>
+    <hyperlink ref="B186" r:id="rId167"/>
+    <hyperlink ref="B187" r:id="rId168"/>
+    <hyperlink ref="B188" r:id="rId169"/>
+    <hyperlink ref="B189" r:id="rId170"/>
+    <hyperlink ref="B190" r:id="rId171"/>
+    <hyperlink ref="B191" r:id="rId172"/>
+    <hyperlink ref="B192" r:id="rId173"/>
+    <hyperlink ref="B193" r:id="rId174"/>
+    <hyperlink ref="B194" r:id="rId175"/>
+    <hyperlink ref="B195" r:id="rId176"/>
+    <hyperlink ref="B196" r:id="rId177"/>
+    <hyperlink ref="B197" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B198" r:id="rId179"/>
+    <hyperlink ref="B199" r:id="rId180"/>
+    <hyperlink ref="B200" r:id="rId181"/>
+    <hyperlink ref="B201" r:id="rId182"/>
+    <hyperlink ref="B202" r:id="rId183"/>
+    <hyperlink ref="B203" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B204" r:id="rId185"/>
+    <hyperlink ref="B205" r:id="rId186"/>
+    <hyperlink ref="B206" r:id="rId187"/>
+    <hyperlink ref="B207" r:id="rId188"/>
+    <hyperlink ref="B208" r:id="rId189"/>
+    <hyperlink ref="B209" r:id="rId190"/>
+    <hyperlink ref="B210" r:id="rId191"/>
+    <hyperlink ref="B211" r:id="rId192"/>
+    <hyperlink ref="B214" r:id="rId193"/>
+    <hyperlink ref="B215" r:id="rId194"/>
+    <hyperlink ref="B216" r:id="rId195"/>
+    <hyperlink ref="B217" r:id="rId196"/>
+    <hyperlink ref="B218" r:id="rId197"/>
+    <hyperlink ref="B219" r:id="rId198"/>
+    <hyperlink ref="B220" r:id="rId199"/>
+    <hyperlink ref="B221" r:id="rId200"/>
+    <hyperlink ref="B222" r:id="rId201"/>
+    <hyperlink ref="B223" r:id="rId202"/>
+    <hyperlink ref="B224" r:id="rId203"/>
+    <hyperlink ref="B225" r:id="rId204"/>
+    <hyperlink ref="B226" r:id="rId205"/>
+    <hyperlink ref="B227" r:id="rId206"/>
+    <hyperlink ref="B228" r:id="rId207"/>
+    <hyperlink ref="B229" r:id="rId208"/>
+    <hyperlink ref="B230" r:id="rId209"/>
+    <hyperlink ref="B231" r:id="rId210"/>
+    <hyperlink ref="B232" r:id="rId211"/>
+    <hyperlink ref="B233" r:id="rId212"/>
+    <hyperlink ref="B234" r:id="rId213"/>
+    <hyperlink ref="B235" r:id="rId214"/>
+    <hyperlink ref="B238" r:id="rId215"/>
+    <hyperlink ref="B239" r:id="rId216"/>
+    <hyperlink ref="B240" r:id="rId217"/>
+    <hyperlink ref="B241" r:id="rId218"/>
+    <hyperlink ref="B242" r:id="rId219"/>
+    <hyperlink ref="B243" r:id="rId220"/>
+    <hyperlink ref="B244" r:id="rId221"/>
+    <hyperlink ref="B245" r:id="rId222"/>
+    <hyperlink ref="B246" r:id="rId223"/>
+    <hyperlink ref="B247" r:id="rId224"/>
+    <hyperlink ref="B248" r:id="rId225"/>
+    <hyperlink ref="B249" r:id="rId226"/>
+    <hyperlink ref="B250" r:id="rId227"/>
+    <hyperlink ref="B251" r:id="rId228"/>
+    <hyperlink ref="B252" r:id="rId229"/>
+    <hyperlink ref="B253" r:id="rId230"/>
+    <hyperlink ref="B254" r:id="rId231"/>
+    <hyperlink ref="B255" r:id="rId232"/>
+    <hyperlink ref="B256" r:id="rId233"/>
+    <hyperlink ref="B257" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B258" r:id="rId235"/>
+    <hyperlink ref="B259" r:id="rId236"/>
+    <hyperlink ref="B260" r:id="rId237"/>
+    <hyperlink ref="B261" r:id="rId238"/>
+    <hyperlink ref="B262" r:id="rId239"/>
+    <hyperlink ref="B263" r:id="rId240"/>
+    <hyperlink ref="B264" r:id="rId241"/>
+    <hyperlink ref="B265" r:id="rId242"/>
+    <hyperlink ref="B266" r:id="rId243"/>
+    <hyperlink ref="B267" r:id="rId244"/>
+    <hyperlink ref="B268" r:id="rId245"/>
+    <hyperlink ref="B269" r:id="rId246"/>
+    <hyperlink ref="B270" r:id="rId247"/>
+    <hyperlink ref="B271" r:id="rId248"/>
+    <hyperlink ref="B272" r:id="rId249"/>
+    <hyperlink ref="B275" r:id="rId250"/>
+    <hyperlink ref="B276" r:id="rId251"/>
+    <hyperlink ref="B277" r:id="rId252"/>
+    <hyperlink ref="B278" r:id="rId253"/>
+    <hyperlink ref="B279" r:id="rId254"/>
+    <hyperlink ref="B280" r:id="rId255"/>
+    <hyperlink ref="B281" r:id="rId256"/>
+    <hyperlink ref="B282" r:id="rId257"/>
+    <hyperlink ref="B283" r:id="rId258"/>
+    <hyperlink ref="B284" r:id="rId259"/>
+    <hyperlink ref="B285" r:id="rId260"/>
+    <hyperlink ref="B286" r:id="rId261"/>
+    <hyperlink ref="B287" r:id="rId262"/>
+    <hyperlink ref="B288" r:id="rId263"/>
+    <hyperlink ref="B289" r:id="rId264"/>
+    <hyperlink ref="B290" r:id="rId265"/>
+    <hyperlink ref="B291" r:id="rId266"/>
+    <hyperlink ref="B292" r:id="rId267"/>
+    <hyperlink ref="B293" r:id="rId268"/>
+    <hyperlink ref="B296" r:id="rId269"/>
+    <hyperlink ref="B297" r:id="rId270"/>
+    <hyperlink ref="B298" r:id="rId271"/>
+    <hyperlink ref="B299" r:id="rId272"/>
+    <hyperlink ref="B300" r:id="rId273"/>
+    <hyperlink ref="B301" r:id="rId274"/>
+    <hyperlink ref="B302" r:id="rId275"/>
+    <hyperlink ref="B303" r:id="rId276"/>
+    <hyperlink ref="B304" r:id="rId277"/>
+    <hyperlink ref="B305" r:id="rId278"/>
+    <hyperlink ref="B306" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId280"/>
+    <hyperlink ref="B308" r:id="rId281"/>
+    <hyperlink ref="B309" r:id="rId282"/>
+    <hyperlink ref="B310" r:id="rId283"/>
+    <hyperlink ref="B311" r:id="rId284"/>
+    <hyperlink ref="B312" r:id="rId285"/>
+    <hyperlink ref="B313" r:id="rId286"/>
+    <hyperlink ref="B314" r:id="rId287"/>
+    <hyperlink ref="B315" r:id="rId288"/>
+    <hyperlink ref="B316" r:id="rId289"/>
+    <hyperlink ref="B317" r:id="rId290"/>
+    <hyperlink ref="B318" r:id="rId291"/>
+    <hyperlink ref="B319" r:id="rId292"/>
+    <hyperlink ref="B320" r:id="rId293"/>
+    <hyperlink ref="B321" r:id="rId294"/>
+    <hyperlink ref="B322" r:id="rId295"/>
+    <hyperlink ref="B323" r:id="rId296"/>
+    <hyperlink ref="B324" r:id="rId297"/>
+    <hyperlink ref="B325" r:id="rId298"/>
+    <hyperlink ref="B326" r:id="rId299"/>
+    <hyperlink ref="B327" r:id="rId300"/>
+    <hyperlink ref="B328" r:id="rId301"/>
+    <hyperlink ref="B329" r:id="rId302"/>
+    <hyperlink ref="B330" r:id="rId303"/>
+    <hyperlink ref="B331" r:id="rId304"/>
+    <hyperlink ref="B332" r:id="rId305"/>
+    <hyperlink ref="B333" r:id="rId306"/>
+    <hyperlink ref="B336" r:id="rId307"/>
+    <hyperlink ref="B337" r:id="rId308"/>
+    <hyperlink ref="B338" r:id="rId309"/>
+    <hyperlink ref="B339" r:id="rId310"/>
+    <hyperlink ref="B340" r:id="rId311"/>
+    <hyperlink ref="B341" r:id="rId312"/>
+    <hyperlink ref="B342" r:id="rId313"/>
+    <hyperlink ref="B343" r:id="rId314"/>
+    <hyperlink ref="B344" r:id="rId315"/>
+    <hyperlink ref="B345" r:id="rId316"/>
+    <hyperlink ref="B346" r:id="rId317"/>
+    <hyperlink ref="B347" r:id="rId318"/>
+    <hyperlink ref="B348" r:id="rId319"/>
+    <hyperlink ref="B349" r:id="rId320"/>
+    <hyperlink ref="B350" r:id="rId321"/>
+    <hyperlink ref="B351" r:id="rId322"/>
+    <hyperlink ref="B352" r:id="rId323"/>
+    <hyperlink ref="B353" r:id="rId324"/>
+    <hyperlink ref="B357" r:id="rId325"/>
+    <hyperlink ref="B358" r:id="rId326"/>
+    <hyperlink ref="B359" r:id="rId327"/>
+    <hyperlink ref="B360" r:id="rId328"/>
+    <hyperlink ref="B361" r:id="rId329"/>
+    <hyperlink ref="B362" r:id="rId330"/>
+    <hyperlink ref="B363" r:id="rId331"/>
+    <hyperlink ref="B364" r:id="rId332"/>
+    <hyperlink ref="B365" r:id="rId333"/>
+    <hyperlink ref="B366" r:id="rId334"/>
+    <hyperlink ref="B367" r:id="rId335"/>
+    <hyperlink ref="B368" r:id="rId336"/>
+    <hyperlink ref="B369" r:id="rId337"/>
+    <hyperlink ref="B370" r:id="rId338"/>
+    <hyperlink ref="B371" r:id="rId339"/>
+    <hyperlink ref="B372" r:id="rId340"/>
+    <hyperlink ref="B373" r:id="rId341"/>
+    <hyperlink ref="B374" r:id="rId342"/>
+    <hyperlink ref="B375" r:id="rId343"/>
+    <hyperlink ref="B376" r:id="rId344"/>
+    <hyperlink ref="B377" r:id="rId345"/>
+    <hyperlink ref="B378" r:id="rId346"/>
+    <hyperlink ref="B379" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId348"/>
+    <hyperlink ref="B381" r:id="rId349"/>
+    <hyperlink ref="B382" r:id="rId350"/>
+    <hyperlink ref="B383" r:id="rId351"/>
+    <hyperlink ref="B384" r:id="rId352"/>
+    <hyperlink ref="B385" r:id="rId353"/>
+    <hyperlink ref="B386" r:id="rId354"/>
+    <hyperlink ref="B387" r:id="rId355"/>
+    <hyperlink ref="B388" r:id="rId356"/>
+    <hyperlink ref="B389" r:id="rId357"/>
+    <hyperlink ref="B390" r:id="rId358"/>
+    <hyperlink ref="B391" r:id="rId359"/>
+    <hyperlink ref="B392" r:id="rId360"/>
+    <hyperlink ref="B393" r:id="rId361"/>
+    <hyperlink ref="B394" r:id="rId362"/>
+    <hyperlink ref="B396" r:id="rId363"/>
+    <hyperlink ref="B395" r:id="rId364"/>
+    <hyperlink ref="B397" r:id="rId365"/>
+    <hyperlink ref="B398" r:id="rId366"/>
+    <hyperlink ref="B399" r:id="rId367"/>
+    <hyperlink ref="B402" r:id="rId368"/>
+    <hyperlink ref="B403" r:id="rId369"/>
+    <hyperlink ref="B404" r:id="rId370"/>
+    <hyperlink ref="B405" r:id="rId371"/>
+    <hyperlink ref="B406" r:id="rId372" display="Implement a Phone Directory"/>
+    <hyperlink ref="B407" r:id="rId373"/>
+    <hyperlink ref="B410" r:id="rId374"/>
+    <hyperlink ref="B411" r:id="rId375"/>
+    <hyperlink ref="B412" r:id="rId376"/>
+    <hyperlink ref="B413" r:id="rId377"/>
+    <hyperlink ref="B414" r:id="rId378"/>
+    <hyperlink ref="B415" r:id="rId379"/>
+    <hyperlink ref="B416" r:id="rId380"/>
+    <hyperlink ref="B417" r:id="rId381"/>
+    <hyperlink ref="B418" r:id="rId382"/>
+    <hyperlink ref="B419" r:id="rId383"/>
+    <hyperlink ref="B420" r:id="rId384"/>
+    <hyperlink ref="B421" r:id="rId385"/>
+    <hyperlink ref="B422" r:id="rId386"/>
+    <hyperlink ref="B423" r:id="rId387"/>
+    <hyperlink ref="B424" r:id="rId388"/>
+    <hyperlink ref="B425" r:id="rId389"/>
+    <hyperlink ref="B426" r:id="rId390"/>
+    <hyperlink ref="B427" r:id="rId391"/>
+    <hyperlink ref="B428" r:id="rId392"/>
+    <hyperlink ref="B429" r:id="rId393"/>
+    <hyperlink ref="B430" r:id="rId394"/>
+    <hyperlink ref="B431" r:id="rId395"/>
+    <hyperlink ref="B432" r:id="rId396"/>
+    <hyperlink ref="B433" r:id="rId397"/>
+    <hyperlink ref="B434" r:id="rId398"/>
+    <hyperlink ref="B435" r:id="rId399"/>
+    <hyperlink ref="B436" r:id="rId400"/>
+    <hyperlink ref="B437" r:id="rId401"/>
+    <hyperlink ref="B438" r:id="rId402"/>
+    <hyperlink ref="B439" r:id="rId403"/>
+    <hyperlink ref="B440" r:id="rId404"/>
+    <hyperlink ref="B441" r:id="rId405"/>
+    <hyperlink ref="B442" r:id="rId406"/>
+    <hyperlink ref="B443" r:id="rId407"/>
+    <hyperlink ref="B444" r:id="rId408"/>
+    <hyperlink ref="B445" r:id="rId409"/>
+    <hyperlink ref="B446" r:id="rId410"/>
+    <hyperlink ref="B447" r:id="rId411"/>
+    <hyperlink ref="B448" r:id="rId412"/>
+    <hyperlink ref="B449" r:id="rId413"/>
+    <hyperlink ref="B451" r:id="rId414"/>
+    <hyperlink ref="B450" r:id="rId415"/>
+    <hyperlink ref="B452" r:id="rId416"/>
+    <hyperlink ref="B453" r:id="rId417"/>
+    <hyperlink ref="B454" r:id="rId418"/>
+    <hyperlink ref="B455" r:id="rId419"/>
+    <hyperlink ref="B456" r:id="rId420"/>
+    <hyperlink ref="B457" r:id="rId421"/>
+    <hyperlink ref="B458" r:id="rId422"/>
+    <hyperlink ref="B459" r:id="rId423"/>
+    <hyperlink ref="B460" r:id="rId424"/>
+    <hyperlink ref="B461" r:id="rId425"/>
+    <hyperlink ref="B462" r:id="rId426"/>
+    <hyperlink ref="B469" r:id="rId427"/>
+    <hyperlink ref="B468" r:id="rId428"/>
+    <hyperlink ref="B467" r:id="rId429"/>
+    <hyperlink ref="B466" r:id="rId430"/>
+    <hyperlink ref="B465" r:id="rId431"/>
+    <hyperlink ref="B464" r:id="rId432"/>
+    <hyperlink ref="B463" r:id="rId433"/>
+    <hyperlink ref="B472" r:id="rId434"/>
+    <hyperlink ref="B473" r:id="rId435"/>
+    <hyperlink ref="B474" r:id="rId436"/>
+    <hyperlink ref="B475" r:id="rId437"/>
+    <hyperlink ref="B476" r:id="rId438"/>
+    <hyperlink ref="B477" r:id="rId439"/>
+    <hyperlink ref="B478" r:id="rId440"/>
+    <hyperlink ref="B481" r:id="rId441"/>
+    <hyperlink ref="B479" r:id="rId442"/>
+    <hyperlink ref="B480" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId444"/>
+    <hyperlink ref="B2" r:id="rId445"/>
+    <hyperlink ref="B71" r:id="rId446"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
solved some more string questions
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2642,7 +2642,7 @@
         <v>73</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="21">
@@ -2664,7 +2664,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="21">
@@ -2675,7 +2675,7 @@
         <v>76</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="21">
@@ -2686,7 +2686,7 @@
         <v>77</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="21">
@@ -6615,7 +6615,7 @@
         <v>433</v>
       </c>
       <c r="C451" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="452" spans="1:3" ht="21">

</xml_diff>

<commit_message>
added some codes and pdfs
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2697,7 +2697,7 @@
         <v>78</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="21">
@@ -2708,7 +2708,7 @@
         <v>79</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="21">
@@ -2719,7 +2719,7 @@
         <v>80</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="21">
@@ -2730,7 +2730,7 @@
         <v>81</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="21">
@@ -2741,7 +2741,7 @@
         <v>82</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="21">
@@ -2785,7 +2785,7 @@
         <v>86</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="21">
@@ -2796,7 +2796,7 @@
         <v>87</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="21">
@@ -2807,7 +2807,7 @@
         <v>88</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="21">
@@ -2818,7 +2818,7 @@
         <v>89</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="21">
@@ -2829,7 +2829,7 @@
         <v>90</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="21">
@@ -2840,7 +2840,7 @@
         <v>91</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="21">
@@ -2851,7 +2851,7 @@
         <v>92</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="21">
@@ -2862,7 +2862,7 @@
         <v>93</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="21">
@@ -2873,7 +2873,7 @@
         <v>94</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="21">
@@ -2895,7 +2895,7 @@
         <v>96</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="21">
@@ -4686,7 +4686,7 @@
         <v>261</v>
       </c>
       <c r="C268" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="269" spans="1:3" ht="21">
@@ -4719,7 +4719,7 @@
         <v>87</v>
       </c>
       <c r="C271" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="272" spans="1:3" ht="21">
@@ -4730,7 +4730,7 @@
         <v>264</v>
       </c>
       <c r="C272" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="273" spans="1:3" ht="21">
@@ -5425,7 +5425,7 @@
         <v>328</v>
       </c>
       <c r="C339" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="340" spans="1:3" ht="21">
@@ -5447,7 +5447,7 @@
         <v>330</v>
       </c>
       <c r="C341" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="342" spans="1:3" ht="21">
@@ -5458,7 +5458,7 @@
         <v>331</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="343" spans="1:3" ht="21">
@@ -5491,7 +5491,7 @@
         <v>334</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="346" spans="1:3" ht="21">
@@ -5502,7 +5502,7 @@
         <v>335</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="347" spans="1:3" ht="21">
@@ -5513,7 +5513,7 @@
         <v>336</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="348" spans="1:3" ht="21">
@@ -5524,7 +5524,7 @@
         <v>337</v>
       </c>
       <c r="C348" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="21">
@@ -5535,7 +5535,7 @@
         <v>338</v>
       </c>
       <c r="C349" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="350" spans="1:3" ht="21">
@@ -5557,7 +5557,7 @@
         <v>340</v>
       </c>
       <c r="C351" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="352" spans="1:3" ht="21">
@@ -5568,7 +5568,7 @@
         <v>341</v>
       </c>
       <c r="C352" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="353" spans="1:3" ht="21">
@@ -5579,7 +5579,7 @@
         <v>342</v>
       </c>
       <c r="C353" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="354" spans="1:3" ht="21">
@@ -5598,7 +5598,7 @@
         <v>344</v>
       </c>
       <c r="C356" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="21">
@@ -5631,7 +5631,7 @@
         <v>347</v>
       </c>
       <c r="C359" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="360" spans="1:3" ht="21">
@@ -5642,7 +5642,7 @@
         <v>348</v>
       </c>
       <c r="C360" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="361" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Completed heap and added some resources
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B338" sqref="B338"/>
+    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B355" sqref="B355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5392,7 +5392,7 @@
         <v>325</v>
       </c>
       <c r="C336" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="337" spans="1:3" ht="21">
@@ -5403,7 +5403,7 @@
         <v>326</v>
       </c>
       <c r="C337" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="21">
@@ -5414,7 +5414,7 @@
         <v>327</v>
       </c>
       <c r="C338" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="339" spans="1:3" ht="21">
@@ -5436,7 +5436,7 @@
         <v>329</v>
       </c>
       <c r="C340" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="341" spans="1:3" ht="21">
@@ -5469,7 +5469,7 @@
         <v>332</v>
       </c>
       <c r="C343" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="344" spans="1:3" ht="21">
@@ -5480,7 +5480,7 @@
         <v>333</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="345" spans="1:3" ht="21">
@@ -5546,7 +5546,7 @@
         <v>339</v>
       </c>
       <c r="C350" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="351" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved some more questions in Graph
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B355" sqref="B355"/>
+    <sheetView tabSelected="1" topLeftCell="A354" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C365" sqref="C365"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5697,7 +5697,7 @@
         <v>353</v>
       </c>
       <c r="C365" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="21">
@@ -5719,7 +5719,7 @@
         <v>355</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="368" spans="1:3" ht="21">
@@ -5730,7 +5730,7 @@
         <v>356</v>
       </c>
       <c r="C368" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="369" spans="1:3" ht="21">

</xml_diff>

<commit_message>
created a UI for check
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C365" sqref="C365"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3975,7 +3975,7 @@
         <v>196</v>
       </c>
       <c r="C201" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="202" spans="1:3" ht="21">
@@ -4227,7 +4227,7 @@
         <v>219</v>
       </c>
       <c r="C225" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="21">
@@ -4238,7 +4238,7 @@
         <v>220</v>
       </c>
       <c r="C226" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="21">
@@ -4271,7 +4271,7 @@
         <v>223</v>
       </c>
       <c r="C229" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="230" spans="1:3" ht="21">
@@ -4749,7 +4749,7 @@
         <v>266</v>
       </c>
       <c r="C275" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="21">
@@ -4892,7 +4892,7 @@
         <v>279</v>
       </c>
       <c r="C288" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="289" spans="1:3" ht="21">
@@ -5098,7 +5098,7 @@
         <v>298</v>
       </c>
       <c r="C308" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="21">
@@ -5175,7 +5175,7 @@
         <v>305</v>
       </c>
       <c r="C315" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="316" spans="1:3" ht="21">
@@ -5208,7 +5208,7 @@
         <v>308</v>
       </c>
       <c r="C318" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="319" spans="1:3" ht="21">
@@ -5252,7 +5252,7 @@
         <v>312</v>
       </c>
       <c r="C322" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="21">
@@ -5263,7 +5263,7 @@
         <v>313</v>
       </c>
       <c r="C323" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="324" spans="1:3" ht="21">
@@ -5653,7 +5653,7 @@
         <v>349</v>
       </c>
       <c r="C361" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="362" spans="1:3" ht="21">
@@ -5664,7 +5664,7 @@
         <v>350</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="363" spans="1:3" ht="21">
@@ -5906,7 +5906,7 @@
         <v>372</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="385" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Solved one question in BST
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C201" sqref="C201"/>
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C235" sqref="C235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4085,7 +4085,7 @@
         <v>206</v>
       </c>
       <c r="C211" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="212" spans="1:3" ht="21">
@@ -4337,7 +4337,7 @@
         <v>229</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="236" spans="1:3" ht="21">
@@ -5153,7 +5153,7 @@
         <v>303</v>
       </c>
       <c r="C313" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="314" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Changed code for CounterHTML
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A296" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D300" sqref="D300"/>
+    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C276" sqref="C276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4760,7 +4760,7 @@
         <v>267</v>
       </c>
       <c r="C276" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some question for Sapients challenge
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C276" sqref="C276"/>
+    <sheetView tabSelected="1" topLeftCell="A362" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C382" sqref="C382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -5884,7 +5884,7 @@
         <v>370</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="383" spans="1:3" ht="21">

</xml_diff>

<commit_message>
completed searching and sorting
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1855,7 +1855,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3115,7 +3115,7 @@
         <v>117</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="21">
@@ -3236,7 +3236,7 @@
         <v>128</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="21">
@@ -3247,7 +3247,7 @@
         <v>129</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="21">
@@ -3269,7 +3269,7 @@
         <v>131</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="135" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved some LL and DP probs
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3317,7 +3317,7 @@
         <v>136</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="21">
@@ -3328,7 +3328,7 @@
         <v>137</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="21">
@@ -3361,7 +3361,7 @@
         <v>140</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="21">
@@ -3372,7 +3372,7 @@
         <v>141</v>
       </c>
       <c r="C145" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="21">
@@ -6181,7 +6181,7 @@
         <v>395</v>
       </c>
       <c r="C412" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="413" spans="1:3" ht="21">
@@ -6192,7 +6192,7 @@
         <v>396</v>
       </c>
       <c r="C413" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="414" spans="1:3" ht="21">
@@ -6236,7 +6236,7 @@
         <v>273</v>
       </c>
       <c r="C417" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="418" spans="1:3" ht="21">
@@ -6247,7 +6247,7 @@
         <v>400</v>
       </c>
       <c r="C418" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="419" spans="1:3" ht="21">
@@ -6280,7 +6280,7 @@
         <v>403</v>
       </c>
       <c r="C421" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="422" spans="1:3" ht="21">
@@ -6291,7 +6291,7 @@
         <v>404</v>
       </c>
       <c r="C422" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="423" spans="1:3" ht="21">

</xml_diff>

<commit_message>
solved 2 questions of DP
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1865,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B468" sqref="B468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -6313,7 +6313,7 @@
         <v>406</v>
       </c>
       <c r="C424" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="425" spans="1:3" ht="21">
@@ -6324,7 +6324,7 @@
         <v>407</v>
       </c>
       <c r="C425" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="426" spans="1:3" ht="21">
@@ -6335,7 +6335,7 @@
         <v>408</v>
       </c>
       <c r="C426" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="427" spans="1:3" ht="21">
@@ -6357,7 +6357,7 @@
         <v>410</v>
       </c>
       <c r="C428" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="429" spans="1:3" ht="21">
@@ -6368,7 +6368,7 @@
         <v>411</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="430" spans="1:3" ht="21">
@@ -6379,7 +6379,7 @@
         <v>412</v>
       </c>
       <c r="C430" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="431" spans="1:3" ht="21">
@@ -6390,7 +6390,7 @@
         <v>413</v>
       </c>
       <c r="C431" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="432" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Completed stacks and Queues
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tasks\Coding_practice\Final 450\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="1110"/>
   </bookViews>
@@ -10,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -1428,7 +1433,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9">
     <font>
       <sz val="12"/>
@@ -1855,18 +1860,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A449" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B468" sqref="B468"/>
+    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C327" sqref="C327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4582,7 +4587,7 @@
         <v>252</v>
       </c>
       <c r="C259" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="21">
@@ -5137,7 +5142,7 @@
         <v>302</v>
       </c>
       <c r="C312" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="313" spans="1:3" ht="21">
@@ -5192,7 +5197,7 @@
         <v>307</v>
       </c>
       <c r="C317" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="21">
@@ -5214,7 +5219,7 @@
         <v>309</v>
       </c>
       <c r="C319" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="21">
@@ -5225,7 +5230,7 @@
         <v>310</v>
       </c>
       <c r="C320" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="21">
@@ -5236,7 +5241,7 @@
         <v>311</v>
       </c>
       <c r="C321" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="322" spans="1:3" ht="21">
@@ -5269,7 +5274,7 @@
         <v>314</v>
       </c>
       <c r="C324" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="325" spans="1:3" ht="21">
@@ -5280,7 +5285,7 @@
         <v>315</v>
       </c>
       <c r="C325" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="326" spans="1:3" ht="21">
@@ -5291,7 +5296,7 @@
         <v>316</v>
       </c>
       <c r="C326" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="327" spans="1:3" ht="21">
@@ -5302,7 +5307,7 @@
         <v>317</v>
       </c>
       <c r="C327" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="328" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Almost done with linkedList
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C327" sqref="C327"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3344,7 +3344,7 @@
         <v>138</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="21">
@@ -3355,7 +3355,7 @@
         <v>139</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="144" spans="1:3" ht="21">
@@ -3388,7 +3388,7 @@
         <v>142</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="21">
@@ -3399,7 +3399,7 @@
         <v>143</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="21">
@@ -3410,7 +3410,7 @@
         <v>144</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="21">
@@ -3421,7 +3421,7 @@
         <v>145</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="21">
@@ -3432,7 +3432,7 @@
         <v>146</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="21">
@@ -3443,7 +3443,7 @@
         <v>147</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="21">
@@ -3454,7 +3454,7 @@
         <v>148</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="21">
@@ -3465,7 +3465,7 @@
         <v>149</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="21">
@@ -3476,7 +3476,7 @@
         <v>150</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="21">
@@ -3487,7 +3487,7 @@
         <v>151</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="21">
@@ -3608,7 +3608,7 @@
         <v>162</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="21">
@@ -3619,7 +3619,7 @@
         <v>163</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="21">
@@ -7060,330 +7060,330 @@
     <hyperlink ref="B136" r:id="rId121"/>
     <hyperlink ref="B105" r:id="rId122"/>
     <hyperlink ref="B112" r:id="rId123"/>
-    <hyperlink ref="B139" r:id="rId124"/>
-    <hyperlink ref="B140" r:id="rId125"/>
-    <hyperlink ref="B141" r:id="rId126"/>
-    <hyperlink ref="B142" r:id="rId127"/>
-    <hyperlink ref="B143" r:id="rId128"/>
-    <hyperlink ref="B144" r:id="rId129"/>
-    <hyperlink ref="B145" r:id="rId130"/>
-    <hyperlink ref="B146" r:id="rId131"/>
-    <hyperlink ref="B147" r:id="rId132"/>
-    <hyperlink ref="B148" r:id="rId133"/>
-    <hyperlink ref="B149" r:id="rId134"/>
-    <hyperlink ref="B150" r:id="rId135"/>
-    <hyperlink ref="B151" r:id="rId136"/>
-    <hyperlink ref="B152" r:id="rId137"/>
-    <hyperlink ref="B153" r:id="rId138"/>
-    <hyperlink ref="B154" r:id="rId139"/>
-    <hyperlink ref="B155" r:id="rId140"/>
-    <hyperlink ref="B156" r:id="rId141"/>
-    <hyperlink ref="B157" r:id="rId142"/>
-    <hyperlink ref="B158" r:id="rId143"/>
-    <hyperlink ref="B159" r:id="rId144"/>
-    <hyperlink ref="B160" r:id="rId145"/>
-    <hyperlink ref="B161" r:id="rId146"/>
-    <hyperlink ref="B162" r:id="rId147"/>
-    <hyperlink ref="B163" r:id="rId148"/>
-    <hyperlink ref="B166" r:id="rId149"/>
-    <hyperlink ref="B167" r:id="rId150"/>
-    <hyperlink ref="B168" r:id="rId151"/>
-    <hyperlink ref="B169" r:id="rId152"/>
-    <hyperlink ref="B170" r:id="rId153"/>
-    <hyperlink ref="B171" r:id="rId154"/>
-    <hyperlink ref="B172" r:id="rId155"/>
-    <hyperlink ref="B173" r:id="rId156"/>
-    <hyperlink ref="B174" r:id="rId157"/>
-    <hyperlink ref="B177" r:id="rId158"/>
-    <hyperlink ref="B178" r:id="rId159"/>
-    <hyperlink ref="B179" r:id="rId160"/>
-    <hyperlink ref="B180" r:id="rId161"/>
-    <hyperlink ref="B181" r:id="rId162"/>
-    <hyperlink ref="B182" r:id="rId163"/>
-    <hyperlink ref="B183" r:id="rId164"/>
-    <hyperlink ref="B184" r:id="rId165"/>
-    <hyperlink ref="B185" r:id="rId166"/>
-    <hyperlink ref="B186" r:id="rId167"/>
-    <hyperlink ref="B187" r:id="rId168"/>
-    <hyperlink ref="B188" r:id="rId169"/>
-    <hyperlink ref="B189" r:id="rId170"/>
-    <hyperlink ref="B190" r:id="rId171"/>
-    <hyperlink ref="B191" r:id="rId172"/>
-    <hyperlink ref="B192" r:id="rId173"/>
-    <hyperlink ref="B193" r:id="rId174"/>
-    <hyperlink ref="B194" r:id="rId175"/>
-    <hyperlink ref="B195" r:id="rId176"/>
-    <hyperlink ref="B196" r:id="rId177"/>
-    <hyperlink ref="B197" r:id="rId178" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
-    <hyperlink ref="B198" r:id="rId179"/>
-    <hyperlink ref="B199" r:id="rId180"/>
-    <hyperlink ref="B200" r:id="rId181"/>
-    <hyperlink ref="B201" r:id="rId182"/>
-    <hyperlink ref="B202" r:id="rId183"/>
-    <hyperlink ref="B203" r:id="rId184" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
-    <hyperlink ref="B204" r:id="rId185"/>
-    <hyperlink ref="B205" r:id="rId186"/>
-    <hyperlink ref="B206" r:id="rId187"/>
-    <hyperlink ref="B207" r:id="rId188"/>
-    <hyperlink ref="B208" r:id="rId189"/>
-    <hyperlink ref="B209" r:id="rId190"/>
-    <hyperlink ref="B210" r:id="rId191"/>
-    <hyperlink ref="B211" r:id="rId192"/>
-    <hyperlink ref="B214" r:id="rId193"/>
-    <hyperlink ref="B215" r:id="rId194"/>
-    <hyperlink ref="B216" r:id="rId195"/>
-    <hyperlink ref="B217" r:id="rId196"/>
-    <hyperlink ref="B218" r:id="rId197"/>
-    <hyperlink ref="B219" r:id="rId198"/>
-    <hyperlink ref="B220" r:id="rId199"/>
-    <hyperlink ref="B221" r:id="rId200"/>
-    <hyperlink ref="B222" r:id="rId201"/>
-    <hyperlink ref="B223" r:id="rId202"/>
-    <hyperlink ref="B224" r:id="rId203"/>
-    <hyperlink ref="B225" r:id="rId204"/>
-    <hyperlink ref="B226" r:id="rId205"/>
-    <hyperlink ref="B227" r:id="rId206"/>
-    <hyperlink ref="B228" r:id="rId207"/>
-    <hyperlink ref="B229" r:id="rId208"/>
-    <hyperlink ref="B230" r:id="rId209"/>
-    <hyperlink ref="B231" r:id="rId210"/>
-    <hyperlink ref="B232" r:id="rId211"/>
-    <hyperlink ref="B233" r:id="rId212"/>
-    <hyperlink ref="B234" r:id="rId213"/>
-    <hyperlink ref="B235" r:id="rId214"/>
-    <hyperlink ref="B238" r:id="rId215"/>
-    <hyperlink ref="B239" r:id="rId216"/>
-    <hyperlink ref="B240" r:id="rId217"/>
-    <hyperlink ref="B241" r:id="rId218"/>
-    <hyperlink ref="B242" r:id="rId219"/>
-    <hyperlink ref="B243" r:id="rId220"/>
-    <hyperlink ref="B244" r:id="rId221"/>
-    <hyperlink ref="B245" r:id="rId222"/>
-    <hyperlink ref="B246" r:id="rId223"/>
-    <hyperlink ref="B247" r:id="rId224"/>
-    <hyperlink ref="B248" r:id="rId225"/>
-    <hyperlink ref="B249" r:id="rId226"/>
-    <hyperlink ref="B250" r:id="rId227"/>
-    <hyperlink ref="B251" r:id="rId228"/>
-    <hyperlink ref="B252" r:id="rId229"/>
-    <hyperlink ref="B253" r:id="rId230"/>
-    <hyperlink ref="B254" r:id="rId231"/>
-    <hyperlink ref="B255" r:id="rId232"/>
-    <hyperlink ref="B256" r:id="rId233"/>
-    <hyperlink ref="B257" r:id="rId234" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
-    <hyperlink ref="B258" r:id="rId235"/>
-    <hyperlink ref="B259" r:id="rId236"/>
-    <hyperlink ref="B260" r:id="rId237"/>
-    <hyperlink ref="B261" r:id="rId238"/>
-    <hyperlink ref="B262" r:id="rId239"/>
-    <hyperlink ref="B263" r:id="rId240"/>
-    <hyperlink ref="B264" r:id="rId241"/>
-    <hyperlink ref="B265" r:id="rId242"/>
-    <hyperlink ref="B266" r:id="rId243"/>
-    <hyperlink ref="B267" r:id="rId244"/>
-    <hyperlink ref="B268" r:id="rId245"/>
-    <hyperlink ref="B269" r:id="rId246"/>
-    <hyperlink ref="B270" r:id="rId247"/>
-    <hyperlink ref="B271" r:id="rId248"/>
-    <hyperlink ref="B272" r:id="rId249"/>
-    <hyperlink ref="B275" r:id="rId250"/>
-    <hyperlink ref="B276" r:id="rId251"/>
-    <hyperlink ref="B277" r:id="rId252"/>
-    <hyperlink ref="B278" r:id="rId253"/>
-    <hyperlink ref="B279" r:id="rId254"/>
-    <hyperlink ref="B280" r:id="rId255"/>
-    <hyperlink ref="B281" r:id="rId256"/>
-    <hyperlink ref="B282" r:id="rId257"/>
-    <hyperlink ref="B283" r:id="rId258"/>
-    <hyperlink ref="B284" r:id="rId259"/>
-    <hyperlink ref="B285" r:id="rId260"/>
-    <hyperlink ref="B286" r:id="rId261"/>
-    <hyperlink ref="B287" r:id="rId262"/>
-    <hyperlink ref="B288" r:id="rId263"/>
-    <hyperlink ref="B289" r:id="rId264"/>
-    <hyperlink ref="B290" r:id="rId265"/>
-    <hyperlink ref="B291" r:id="rId266"/>
-    <hyperlink ref="B292" r:id="rId267"/>
-    <hyperlink ref="B293" r:id="rId268"/>
-    <hyperlink ref="B296" r:id="rId269"/>
-    <hyperlink ref="B297" r:id="rId270"/>
-    <hyperlink ref="B298" r:id="rId271"/>
-    <hyperlink ref="B299" r:id="rId272"/>
-    <hyperlink ref="B300" r:id="rId273"/>
-    <hyperlink ref="B301" r:id="rId274"/>
-    <hyperlink ref="B302" r:id="rId275"/>
-    <hyperlink ref="B303" r:id="rId276"/>
-    <hyperlink ref="B304" r:id="rId277"/>
-    <hyperlink ref="B305" r:id="rId278"/>
-    <hyperlink ref="B306" r:id="rId279" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
-    <hyperlink ref="B307" r:id="rId280"/>
-    <hyperlink ref="B308" r:id="rId281"/>
-    <hyperlink ref="B309" r:id="rId282"/>
-    <hyperlink ref="B310" r:id="rId283"/>
-    <hyperlink ref="B311" r:id="rId284"/>
-    <hyperlink ref="B312" r:id="rId285"/>
-    <hyperlink ref="B313" r:id="rId286"/>
-    <hyperlink ref="B314" r:id="rId287"/>
-    <hyperlink ref="B315" r:id="rId288"/>
-    <hyperlink ref="B316" r:id="rId289"/>
-    <hyperlink ref="B317" r:id="rId290"/>
-    <hyperlink ref="B318" r:id="rId291"/>
-    <hyperlink ref="B319" r:id="rId292"/>
-    <hyperlink ref="B320" r:id="rId293"/>
-    <hyperlink ref="B321" r:id="rId294"/>
-    <hyperlink ref="B322" r:id="rId295"/>
-    <hyperlink ref="B323" r:id="rId296"/>
-    <hyperlink ref="B324" r:id="rId297"/>
-    <hyperlink ref="B325" r:id="rId298"/>
-    <hyperlink ref="B326" r:id="rId299"/>
-    <hyperlink ref="B327" r:id="rId300"/>
-    <hyperlink ref="B328" r:id="rId301"/>
-    <hyperlink ref="B329" r:id="rId302"/>
-    <hyperlink ref="B330" r:id="rId303"/>
-    <hyperlink ref="B331" r:id="rId304"/>
-    <hyperlink ref="B332" r:id="rId305"/>
-    <hyperlink ref="B333" r:id="rId306"/>
-    <hyperlink ref="B336" r:id="rId307"/>
-    <hyperlink ref="B337" r:id="rId308"/>
-    <hyperlink ref="B338" r:id="rId309"/>
-    <hyperlink ref="B339" r:id="rId310"/>
-    <hyperlink ref="B340" r:id="rId311"/>
-    <hyperlink ref="B341" r:id="rId312"/>
-    <hyperlink ref="B342" r:id="rId313"/>
-    <hyperlink ref="B343" r:id="rId314"/>
-    <hyperlink ref="B344" r:id="rId315"/>
-    <hyperlink ref="B345" r:id="rId316"/>
-    <hyperlink ref="B346" r:id="rId317"/>
-    <hyperlink ref="B347" r:id="rId318"/>
-    <hyperlink ref="B348" r:id="rId319"/>
-    <hyperlink ref="B349" r:id="rId320"/>
-    <hyperlink ref="B350" r:id="rId321"/>
-    <hyperlink ref="B351" r:id="rId322"/>
-    <hyperlink ref="B352" r:id="rId323"/>
-    <hyperlink ref="B353" r:id="rId324"/>
-    <hyperlink ref="B357" r:id="rId325"/>
-    <hyperlink ref="B358" r:id="rId326"/>
-    <hyperlink ref="B359" r:id="rId327"/>
-    <hyperlink ref="B360" r:id="rId328"/>
-    <hyperlink ref="B361" r:id="rId329"/>
-    <hyperlink ref="B362" r:id="rId330"/>
-    <hyperlink ref="B363" r:id="rId331"/>
-    <hyperlink ref="B364" r:id="rId332"/>
-    <hyperlink ref="B365" r:id="rId333"/>
-    <hyperlink ref="B366" r:id="rId334"/>
-    <hyperlink ref="B367" r:id="rId335"/>
-    <hyperlink ref="B368" r:id="rId336"/>
-    <hyperlink ref="B369" r:id="rId337"/>
-    <hyperlink ref="B370" r:id="rId338"/>
-    <hyperlink ref="B371" r:id="rId339"/>
-    <hyperlink ref="B372" r:id="rId340"/>
-    <hyperlink ref="B373" r:id="rId341"/>
-    <hyperlink ref="B374" r:id="rId342"/>
-    <hyperlink ref="B375" r:id="rId343"/>
-    <hyperlink ref="B376" r:id="rId344"/>
-    <hyperlink ref="B377" r:id="rId345"/>
-    <hyperlink ref="B378" r:id="rId346"/>
-    <hyperlink ref="B379" r:id="rId347" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
-    <hyperlink ref="B380" r:id="rId348"/>
-    <hyperlink ref="B381" r:id="rId349"/>
-    <hyperlink ref="B382" r:id="rId350"/>
-    <hyperlink ref="B383" r:id="rId351"/>
-    <hyperlink ref="B384" r:id="rId352"/>
-    <hyperlink ref="B385" r:id="rId353"/>
-    <hyperlink ref="B386" r:id="rId354"/>
-    <hyperlink ref="B387" r:id="rId355"/>
-    <hyperlink ref="B388" r:id="rId356"/>
-    <hyperlink ref="B389" r:id="rId357"/>
-    <hyperlink ref="B390" r:id="rId358"/>
-    <hyperlink ref="B391" r:id="rId359"/>
-    <hyperlink ref="B392" r:id="rId360"/>
-    <hyperlink ref="B393" r:id="rId361"/>
-    <hyperlink ref="B394" r:id="rId362"/>
-    <hyperlink ref="B396" r:id="rId363"/>
-    <hyperlink ref="B395" r:id="rId364"/>
-    <hyperlink ref="B397" r:id="rId365"/>
-    <hyperlink ref="B398" r:id="rId366"/>
-    <hyperlink ref="B399" r:id="rId367"/>
-    <hyperlink ref="B402" r:id="rId368"/>
-    <hyperlink ref="B403" r:id="rId369"/>
-    <hyperlink ref="B404" r:id="rId370"/>
-    <hyperlink ref="B405" r:id="rId371"/>
-    <hyperlink ref="B406" r:id="rId372" display="Implement a Phone Directory"/>
-    <hyperlink ref="B407" r:id="rId373"/>
-    <hyperlink ref="B410" r:id="rId374"/>
-    <hyperlink ref="B411" r:id="rId375"/>
-    <hyperlink ref="B412" r:id="rId376"/>
-    <hyperlink ref="B413" r:id="rId377"/>
-    <hyperlink ref="B414" r:id="rId378"/>
-    <hyperlink ref="B415" r:id="rId379"/>
-    <hyperlink ref="B416" r:id="rId380"/>
-    <hyperlink ref="B417" r:id="rId381"/>
-    <hyperlink ref="B418" r:id="rId382"/>
-    <hyperlink ref="B419" r:id="rId383"/>
-    <hyperlink ref="B420" r:id="rId384"/>
-    <hyperlink ref="B421" r:id="rId385"/>
-    <hyperlink ref="B422" r:id="rId386"/>
-    <hyperlink ref="B423" r:id="rId387"/>
-    <hyperlink ref="B424" r:id="rId388"/>
-    <hyperlink ref="B425" r:id="rId389"/>
-    <hyperlink ref="B426" r:id="rId390"/>
-    <hyperlink ref="B427" r:id="rId391"/>
-    <hyperlink ref="B428" r:id="rId392"/>
-    <hyperlink ref="B429" r:id="rId393"/>
-    <hyperlink ref="B430" r:id="rId394"/>
-    <hyperlink ref="B431" r:id="rId395"/>
-    <hyperlink ref="B432" r:id="rId396"/>
-    <hyperlink ref="B433" r:id="rId397"/>
-    <hyperlink ref="B434" r:id="rId398"/>
-    <hyperlink ref="B435" r:id="rId399"/>
-    <hyperlink ref="B436" r:id="rId400"/>
-    <hyperlink ref="B437" r:id="rId401"/>
-    <hyperlink ref="B438" r:id="rId402"/>
-    <hyperlink ref="B439" r:id="rId403"/>
-    <hyperlink ref="B440" r:id="rId404"/>
-    <hyperlink ref="B441" r:id="rId405"/>
-    <hyperlink ref="B442" r:id="rId406"/>
-    <hyperlink ref="B443" r:id="rId407"/>
-    <hyperlink ref="B444" r:id="rId408"/>
-    <hyperlink ref="B445" r:id="rId409"/>
-    <hyperlink ref="B446" r:id="rId410"/>
-    <hyperlink ref="B447" r:id="rId411"/>
-    <hyperlink ref="B448" r:id="rId412"/>
-    <hyperlink ref="B449" r:id="rId413"/>
-    <hyperlink ref="B451" r:id="rId414"/>
-    <hyperlink ref="B450" r:id="rId415"/>
-    <hyperlink ref="B452" r:id="rId416"/>
-    <hyperlink ref="B453" r:id="rId417"/>
-    <hyperlink ref="B454" r:id="rId418"/>
-    <hyperlink ref="B455" r:id="rId419"/>
-    <hyperlink ref="B456" r:id="rId420"/>
-    <hyperlink ref="B457" r:id="rId421"/>
-    <hyperlink ref="B458" r:id="rId422"/>
-    <hyperlink ref="B459" r:id="rId423"/>
-    <hyperlink ref="B460" r:id="rId424"/>
-    <hyperlink ref="B461" r:id="rId425"/>
-    <hyperlink ref="B462" r:id="rId426"/>
-    <hyperlink ref="B469" r:id="rId427"/>
-    <hyperlink ref="B468" r:id="rId428"/>
-    <hyperlink ref="B467" r:id="rId429"/>
-    <hyperlink ref="B466" r:id="rId430"/>
-    <hyperlink ref="B465" r:id="rId431"/>
-    <hyperlink ref="B464" r:id="rId432"/>
-    <hyperlink ref="B463" r:id="rId433"/>
-    <hyperlink ref="B472" r:id="rId434"/>
-    <hyperlink ref="B473" r:id="rId435"/>
-    <hyperlink ref="B474" r:id="rId436"/>
-    <hyperlink ref="B475" r:id="rId437"/>
-    <hyperlink ref="B476" r:id="rId438"/>
-    <hyperlink ref="B477" r:id="rId439"/>
-    <hyperlink ref="B478" r:id="rId440"/>
-    <hyperlink ref="B481" r:id="rId441"/>
-    <hyperlink ref="B479" r:id="rId442"/>
-    <hyperlink ref="B480" r:id="rId443" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
-    <hyperlink ref="B356" r:id="rId444"/>
-    <hyperlink ref="B2" r:id="rId445"/>
-    <hyperlink ref="B71" r:id="rId446"/>
-    <hyperlink ref="B59" r:id="rId447" location=":~:text=String%20is%20"/>
+    <hyperlink ref="B298" r:id="rId124"/>
+    <hyperlink ref="B299" r:id="rId125"/>
+    <hyperlink ref="B300" r:id="rId126"/>
+    <hyperlink ref="B301" r:id="rId127"/>
+    <hyperlink ref="B302" r:id="rId128"/>
+    <hyperlink ref="B303" r:id="rId129"/>
+    <hyperlink ref="B304" r:id="rId130"/>
+    <hyperlink ref="B305" r:id="rId131"/>
+    <hyperlink ref="B306" r:id="rId132" location=":~:text=The%20stack%20organization%20is%20very,i.e.%2C%20A%20%2B%20B)."/>
+    <hyperlink ref="B307" r:id="rId133"/>
+    <hyperlink ref="B308" r:id="rId134"/>
+    <hyperlink ref="B309" r:id="rId135"/>
+    <hyperlink ref="B310" r:id="rId136"/>
+    <hyperlink ref="B311" r:id="rId137"/>
+    <hyperlink ref="B312" r:id="rId138"/>
+    <hyperlink ref="B313" r:id="rId139"/>
+    <hyperlink ref="B314" r:id="rId140"/>
+    <hyperlink ref="B315" r:id="rId141"/>
+    <hyperlink ref="B316" r:id="rId142"/>
+    <hyperlink ref="B317" r:id="rId143"/>
+    <hyperlink ref="B318" r:id="rId144"/>
+    <hyperlink ref="B319" r:id="rId145"/>
+    <hyperlink ref="B320" r:id="rId146"/>
+    <hyperlink ref="B321" r:id="rId147"/>
+    <hyperlink ref="B322" r:id="rId148"/>
+    <hyperlink ref="B323" r:id="rId149"/>
+    <hyperlink ref="B324" r:id="rId150"/>
+    <hyperlink ref="B325" r:id="rId151"/>
+    <hyperlink ref="B326" r:id="rId152"/>
+    <hyperlink ref="B327" r:id="rId153"/>
+    <hyperlink ref="B328" r:id="rId154"/>
+    <hyperlink ref="B329" r:id="rId155"/>
+    <hyperlink ref="B330" r:id="rId156"/>
+    <hyperlink ref="B331" r:id="rId157"/>
+    <hyperlink ref="B332" r:id="rId158"/>
+    <hyperlink ref="B333" r:id="rId159"/>
+    <hyperlink ref="B336" r:id="rId160"/>
+    <hyperlink ref="B337" r:id="rId161"/>
+    <hyperlink ref="B338" r:id="rId162"/>
+    <hyperlink ref="B339" r:id="rId163"/>
+    <hyperlink ref="B340" r:id="rId164"/>
+    <hyperlink ref="B341" r:id="rId165"/>
+    <hyperlink ref="B342" r:id="rId166"/>
+    <hyperlink ref="B343" r:id="rId167"/>
+    <hyperlink ref="B344" r:id="rId168"/>
+    <hyperlink ref="B345" r:id="rId169"/>
+    <hyperlink ref="B346" r:id="rId170"/>
+    <hyperlink ref="B347" r:id="rId171"/>
+    <hyperlink ref="B348" r:id="rId172"/>
+    <hyperlink ref="B349" r:id="rId173"/>
+    <hyperlink ref="B350" r:id="rId174"/>
+    <hyperlink ref="B351" r:id="rId175"/>
+    <hyperlink ref="B352" r:id="rId176"/>
+    <hyperlink ref="B353" r:id="rId177"/>
+    <hyperlink ref="B357" r:id="rId178"/>
+    <hyperlink ref="B358" r:id="rId179"/>
+    <hyperlink ref="B359" r:id="rId180"/>
+    <hyperlink ref="B360" r:id="rId181"/>
+    <hyperlink ref="B361" r:id="rId182"/>
+    <hyperlink ref="B362" r:id="rId183"/>
+    <hyperlink ref="B363" r:id="rId184"/>
+    <hyperlink ref="B364" r:id="rId185"/>
+    <hyperlink ref="B365" r:id="rId186"/>
+    <hyperlink ref="B366" r:id="rId187"/>
+    <hyperlink ref="B367" r:id="rId188"/>
+    <hyperlink ref="B368" r:id="rId189"/>
+    <hyperlink ref="B369" r:id="rId190"/>
+    <hyperlink ref="B370" r:id="rId191"/>
+    <hyperlink ref="B371" r:id="rId192"/>
+    <hyperlink ref="B372" r:id="rId193"/>
+    <hyperlink ref="B373" r:id="rId194"/>
+    <hyperlink ref="B374" r:id="rId195"/>
+    <hyperlink ref="B375" r:id="rId196"/>
+    <hyperlink ref="B376" r:id="rId197"/>
+    <hyperlink ref="B377" r:id="rId198"/>
+    <hyperlink ref="B378" r:id="rId199"/>
+    <hyperlink ref="B379" r:id="rId200" location=":~:text=Graph%20coloring%20problem%20is%20to,are%20colored%20using%20same%20color."/>
+    <hyperlink ref="B380" r:id="rId201"/>
+    <hyperlink ref="B381" r:id="rId202"/>
+    <hyperlink ref="B382" r:id="rId203"/>
+    <hyperlink ref="B383" r:id="rId204"/>
+    <hyperlink ref="B384" r:id="rId205"/>
+    <hyperlink ref="B385" r:id="rId206"/>
+    <hyperlink ref="B386" r:id="rId207"/>
+    <hyperlink ref="B387" r:id="rId208"/>
+    <hyperlink ref="B388" r:id="rId209"/>
+    <hyperlink ref="B389" r:id="rId210"/>
+    <hyperlink ref="B390" r:id="rId211"/>
+    <hyperlink ref="B391" r:id="rId212"/>
+    <hyperlink ref="B392" r:id="rId213"/>
+    <hyperlink ref="B393" r:id="rId214"/>
+    <hyperlink ref="B394" r:id="rId215"/>
+    <hyperlink ref="B396" r:id="rId216"/>
+    <hyperlink ref="B395" r:id="rId217"/>
+    <hyperlink ref="B397" r:id="rId218"/>
+    <hyperlink ref="B398" r:id="rId219"/>
+    <hyperlink ref="B399" r:id="rId220"/>
+    <hyperlink ref="B402" r:id="rId221"/>
+    <hyperlink ref="B403" r:id="rId222"/>
+    <hyperlink ref="B404" r:id="rId223"/>
+    <hyperlink ref="B405" r:id="rId224"/>
+    <hyperlink ref="B406" r:id="rId225" display="Implement a Phone Directory"/>
+    <hyperlink ref="B407" r:id="rId226"/>
+    <hyperlink ref="B410" r:id="rId227"/>
+    <hyperlink ref="B411" r:id="rId228"/>
+    <hyperlink ref="B412" r:id="rId229"/>
+    <hyperlink ref="B413" r:id="rId230"/>
+    <hyperlink ref="B414" r:id="rId231"/>
+    <hyperlink ref="B415" r:id="rId232"/>
+    <hyperlink ref="B416" r:id="rId233"/>
+    <hyperlink ref="B417" r:id="rId234"/>
+    <hyperlink ref="B418" r:id="rId235"/>
+    <hyperlink ref="B419" r:id="rId236"/>
+    <hyperlink ref="B420" r:id="rId237"/>
+    <hyperlink ref="B421" r:id="rId238"/>
+    <hyperlink ref="B422" r:id="rId239"/>
+    <hyperlink ref="B423" r:id="rId240"/>
+    <hyperlink ref="B424" r:id="rId241"/>
+    <hyperlink ref="B425" r:id="rId242"/>
+    <hyperlink ref="B426" r:id="rId243"/>
+    <hyperlink ref="B427" r:id="rId244"/>
+    <hyperlink ref="B428" r:id="rId245"/>
+    <hyperlink ref="B429" r:id="rId246"/>
+    <hyperlink ref="B430" r:id="rId247"/>
+    <hyperlink ref="B431" r:id="rId248"/>
+    <hyperlink ref="B432" r:id="rId249"/>
+    <hyperlink ref="B433" r:id="rId250"/>
+    <hyperlink ref="B434" r:id="rId251"/>
+    <hyperlink ref="B435" r:id="rId252"/>
+    <hyperlink ref="B436" r:id="rId253"/>
+    <hyperlink ref="B437" r:id="rId254"/>
+    <hyperlink ref="B438" r:id="rId255"/>
+    <hyperlink ref="B439" r:id="rId256"/>
+    <hyperlink ref="B440" r:id="rId257"/>
+    <hyperlink ref="B441" r:id="rId258"/>
+    <hyperlink ref="B442" r:id="rId259"/>
+    <hyperlink ref="B443" r:id="rId260"/>
+    <hyperlink ref="B444" r:id="rId261"/>
+    <hyperlink ref="B445" r:id="rId262"/>
+    <hyperlink ref="B446" r:id="rId263"/>
+    <hyperlink ref="B447" r:id="rId264"/>
+    <hyperlink ref="B448" r:id="rId265"/>
+    <hyperlink ref="B449" r:id="rId266"/>
+    <hyperlink ref="B451" r:id="rId267"/>
+    <hyperlink ref="B450" r:id="rId268"/>
+    <hyperlink ref="B452" r:id="rId269"/>
+    <hyperlink ref="B453" r:id="rId270"/>
+    <hyperlink ref="B454" r:id="rId271"/>
+    <hyperlink ref="B455" r:id="rId272"/>
+    <hyperlink ref="B456" r:id="rId273"/>
+    <hyperlink ref="B457" r:id="rId274"/>
+    <hyperlink ref="B458" r:id="rId275"/>
+    <hyperlink ref="B459" r:id="rId276"/>
+    <hyperlink ref="B460" r:id="rId277"/>
+    <hyperlink ref="B461" r:id="rId278"/>
+    <hyperlink ref="B462" r:id="rId279"/>
+    <hyperlink ref="B469" r:id="rId280"/>
+    <hyperlink ref="B468" r:id="rId281"/>
+    <hyperlink ref="B467" r:id="rId282"/>
+    <hyperlink ref="B466" r:id="rId283"/>
+    <hyperlink ref="B465" r:id="rId284"/>
+    <hyperlink ref="B464" r:id="rId285"/>
+    <hyperlink ref="B463" r:id="rId286"/>
+    <hyperlink ref="B472" r:id="rId287"/>
+    <hyperlink ref="B473" r:id="rId288"/>
+    <hyperlink ref="B474" r:id="rId289"/>
+    <hyperlink ref="B475" r:id="rId290"/>
+    <hyperlink ref="B476" r:id="rId291"/>
+    <hyperlink ref="B477" r:id="rId292"/>
+    <hyperlink ref="B478" r:id="rId293"/>
+    <hyperlink ref="B481" r:id="rId294"/>
+    <hyperlink ref="B479" r:id="rId295"/>
+    <hyperlink ref="B480" r:id="rId296" location=":~:text=Given%20an%20integer%20n%2C%20calculate,*%2C%20%2F%20and%20pow().&amp;text=A%20Simple%20Solution%20is%20to%20repeatedly%20add%20n%20to%20result."/>
+    <hyperlink ref="B356" r:id="rId297"/>
+    <hyperlink ref="B2" r:id="rId298"/>
+    <hyperlink ref="B71" r:id="rId299"/>
+    <hyperlink ref="B59" r:id="rId300" location=":~:text=String%20is%20"/>
+    <hyperlink ref="B297" r:id="rId301"/>
+    <hyperlink ref="B296" r:id="rId302"/>
+    <hyperlink ref="B293" r:id="rId303"/>
+    <hyperlink ref="B292" r:id="rId304"/>
+    <hyperlink ref="B291" r:id="rId305"/>
+    <hyperlink ref="B290" r:id="rId306"/>
+    <hyperlink ref="B289" r:id="rId307"/>
+    <hyperlink ref="B288" r:id="rId308"/>
+    <hyperlink ref="B287" r:id="rId309"/>
+    <hyperlink ref="B286" r:id="rId310"/>
+    <hyperlink ref="B285" r:id="rId311"/>
+    <hyperlink ref="B284" r:id="rId312"/>
+    <hyperlink ref="B283" r:id="rId313"/>
+    <hyperlink ref="B282" r:id="rId314"/>
+    <hyperlink ref="B281" r:id="rId315"/>
+    <hyperlink ref="B280" r:id="rId316"/>
+    <hyperlink ref="B279" r:id="rId317"/>
+    <hyperlink ref="B278" r:id="rId318"/>
+    <hyperlink ref="B277" r:id="rId319"/>
+    <hyperlink ref="B276" r:id="rId320"/>
+    <hyperlink ref="B275" r:id="rId321"/>
+    <hyperlink ref="B272" r:id="rId322"/>
+    <hyperlink ref="B271" r:id="rId323"/>
+    <hyperlink ref="B270" r:id="rId324"/>
+    <hyperlink ref="B269" r:id="rId325"/>
+    <hyperlink ref="B268" r:id="rId326"/>
+    <hyperlink ref="B267" r:id="rId327"/>
+    <hyperlink ref="B266" r:id="rId328"/>
+    <hyperlink ref="B265" r:id="rId329"/>
+    <hyperlink ref="B264" r:id="rId330"/>
+    <hyperlink ref="B263" r:id="rId331"/>
+    <hyperlink ref="B262" r:id="rId332"/>
+    <hyperlink ref="B261" r:id="rId333"/>
+    <hyperlink ref="B260" r:id="rId334"/>
+    <hyperlink ref="B259" r:id="rId335"/>
+    <hyperlink ref="B258" r:id="rId336"/>
+    <hyperlink ref="B257" r:id="rId337" location=":~:text=It%20consists%20of%20two%20steps,result%20to%20the%20sum%20S."/>
+    <hyperlink ref="B256" r:id="rId338"/>
+    <hyperlink ref="B255" r:id="rId339"/>
+    <hyperlink ref="B254" r:id="rId340"/>
+    <hyperlink ref="B253" r:id="rId341"/>
+    <hyperlink ref="B252" r:id="rId342"/>
+    <hyperlink ref="B251" r:id="rId343"/>
+    <hyperlink ref="B250" r:id="rId344"/>
+    <hyperlink ref="B249" r:id="rId345"/>
+    <hyperlink ref="B248" r:id="rId346"/>
+    <hyperlink ref="B247" r:id="rId347"/>
+    <hyperlink ref="B246" r:id="rId348"/>
+    <hyperlink ref="B245" r:id="rId349"/>
+    <hyperlink ref="B244" r:id="rId350"/>
+    <hyperlink ref="B243" r:id="rId351"/>
+    <hyperlink ref="B242" r:id="rId352"/>
+    <hyperlink ref="B241" r:id="rId353"/>
+    <hyperlink ref="B240" r:id="rId354"/>
+    <hyperlink ref="B239" r:id="rId355"/>
+    <hyperlink ref="B238" r:id="rId356"/>
+    <hyperlink ref="B235" r:id="rId357"/>
+    <hyperlink ref="B234" r:id="rId358"/>
+    <hyperlink ref="B233" r:id="rId359"/>
+    <hyperlink ref="B232" r:id="rId360"/>
+    <hyperlink ref="B231" r:id="rId361"/>
+    <hyperlink ref="B230" r:id="rId362"/>
+    <hyperlink ref="B229" r:id="rId363"/>
+    <hyperlink ref="B228" r:id="rId364"/>
+    <hyperlink ref="B227" r:id="rId365"/>
+    <hyperlink ref="B226" r:id="rId366"/>
+    <hyperlink ref="B225" r:id="rId367"/>
+    <hyperlink ref="B224" r:id="rId368"/>
+    <hyperlink ref="B223" r:id="rId369"/>
+    <hyperlink ref="B222" r:id="rId370"/>
+    <hyperlink ref="B221" r:id="rId371"/>
+    <hyperlink ref="B220" r:id="rId372"/>
+    <hyperlink ref="B219" r:id="rId373"/>
+    <hyperlink ref="B218" r:id="rId374"/>
+    <hyperlink ref="B217" r:id="rId375"/>
+    <hyperlink ref="B216" r:id="rId376"/>
+    <hyperlink ref="B215" r:id="rId377"/>
+    <hyperlink ref="B214" r:id="rId378"/>
+    <hyperlink ref="B211" r:id="rId379"/>
+    <hyperlink ref="B210" r:id="rId380"/>
+    <hyperlink ref="B209" r:id="rId381"/>
+    <hyperlink ref="B208" r:id="rId382"/>
+    <hyperlink ref="B207" r:id="rId383"/>
+    <hyperlink ref="B206" r:id="rId384"/>
+    <hyperlink ref="B205" r:id="rId385"/>
+    <hyperlink ref="B204" r:id="rId386"/>
+    <hyperlink ref="B203" r:id="rId387" location=":~:text=Since%20the%20graph%20is%20undirected,graph%20is%20connected%2C%20otherwise%20not."/>
+    <hyperlink ref="B202" r:id="rId388"/>
+    <hyperlink ref="B201" r:id="rId389"/>
+    <hyperlink ref="B200" r:id="rId390"/>
+    <hyperlink ref="B199" r:id="rId391"/>
+    <hyperlink ref="B198" r:id="rId392"/>
+    <hyperlink ref="B197" r:id="rId393" location=":~:text=Given%20the%20array%20representation%20of,it%20into%20Binary%20Search%20Tree.&amp;text=Swap%201%3A%20Swap%20node%208,node%209%20with%20node%2010."/>
+    <hyperlink ref="B196" r:id="rId394"/>
+    <hyperlink ref="B195" r:id="rId395"/>
+    <hyperlink ref="B194" r:id="rId396"/>
+    <hyperlink ref="B193" r:id="rId397"/>
+    <hyperlink ref="B192" r:id="rId398"/>
+    <hyperlink ref="B191" r:id="rId399"/>
+    <hyperlink ref="B190" r:id="rId400"/>
+    <hyperlink ref="B189" r:id="rId401"/>
+    <hyperlink ref="B188" r:id="rId402"/>
+    <hyperlink ref="B187" r:id="rId403"/>
+    <hyperlink ref="B186" r:id="rId404"/>
+    <hyperlink ref="B185" r:id="rId405"/>
+    <hyperlink ref="B184" r:id="rId406"/>
+    <hyperlink ref="B183" r:id="rId407"/>
+    <hyperlink ref="B182" r:id="rId408"/>
+    <hyperlink ref="B181" r:id="rId409"/>
+    <hyperlink ref="B180" r:id="rId410"/>
+    <hyperlink ref="B179" r:id="rId411"/>
+    <hyperlink ref="B178" r:id="rId412"/>
+    <hyperlink ref="B177" r:id="rId413"/>
+    <hyperlink ref="B174" r:id="rId414"/>
+    <hyperlink ref="B173" r:id="rId415"/>
+    <hyperlink ref="B172" r:id="rId416"/>
+    <hyperlink ref="B171" r:id="rId417"/>
+    <hyperlink ref="B170" r:id="rId418"/>
+    <hyperlink ref="B169" r:id="rId419"/>
+    <hyperlink ref="B168" r:id="rId420"/>
+    <hyperlink ref="B167" r:id="rId421"/>
+    <hyperlink ref="B166" r:id="rId422"/>
+    <hyperlink ref="B163" r:id="rId423"/>
+    <hyperlink ref="B162" r:id="rId424"/>
+    <hyperlink ref="B161" r:id="rId425"/>
+    <hyperlink ref="B160" r:id="rId426"/>
+    <hyperlink ref="B159" r:id="rId427"/>
+    <hyperlink ref="B158" r:id="rId428"/>
+    <hyperlink ref="B157" r:id="rId429"/>
+    <hyperlink ref="B156" r:id="rId430"/>
+    <hyperlink ref="B155" r:id="rId431"/>
+    <hyperlink ref="B154" r:id="rId432"/>
+    <hyperlink ref="B153" r:id="rId433"/>
+    <hyperlink ref="B152" r:id="rId434"/>
+    <hyperlink ref="B151" r:id="rId435"/>
+    <hyperlink ref="B150" r:id="rId436"/>
+    <hyperlink ref="B149" r:id="rId437"/>
+    <hyperlink ref="B148" r:id="rId438"/>
+    <hyperlink ref="B147" r:id="rId439"/>
+    <hyperlink ref="B146" r:id="rId440"/>
+    <hyperlink ref="B145" r:id="rId441"/>
+    <hyperlink ref="B144" r:id="rId442"/>
+    <hyperlink ref="B143" r:id="rId443"/>
+    <hyperlink ref="B142" r:id="rId444"/>
+    <hyperlink ref="B141" r:id="rId445"/>
+    <hyperlink ref="B140" r:id="rId446"/>
+    <hyperlink ref="B139" r:id="rId447"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId448"/>

</xml_diff>

<commit_message>
Solved boundary question of tree
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B168" sqref="B168"/>
+    <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3630,7 +3630,7 @@
         <v>164</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="21">
@@ -3876,7 +3876,7 @@
         <v>187</v>
       </c>
       <c r="C192" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="193" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Almost done with tree remaining 7 questions
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1871,7 +1871,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A188" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C192" sqref="C192"/>
+      <selection activeCell="C201" sqref="C201:C203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3887,7 +3887,7 @@
         <v>188</v>
       </c>
       <c r="C193" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="194" spans="1:3" ht="21">
@@ -3898,7 +3898,7 @@
         <v>189</v>
       </c>
       <c r="C194" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="21">
@@ -3909,7 +3909,7 @@
         <v>190</v>
       </c>
       <c r="C195" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="196" spans="1:3" ht="21">
@@ -3920,7 +3920,7 @@
         <v>191</v>
       </c>
       <c r="C196" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="21">
@@ -3931,7 +3931,7 @@
         <v>192</v>
       </c>
       <c r="C197" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="21">
@@ -3942,7 +3942,7 @@
         <v>193</v>
       </c>
       <c r="C198" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="21">
@@ -3953,7 +3953,7 @@
         <v>194</v>
       </c>
       <c r="C199" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="200" spans="1:3" ht="21">
@@ -3964,7 +3964,7 @@
         <v>195</v>
       </c>
       <c r="C200" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="201" spans="1:3" ht="21">
@@ -3986,7 +3986,7 @@
         <v>197</v>
       </c>
       <c r="C202" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="203" spans="1:3" ht="21">
@@ -3997,7 +3997,7 @@
         <v>198</v>
       </c>
       <c r="C203" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="204" spans="1:3" ht="21">

</xml_diff>

<commit_message>
About to complete greedy
</commit_message>
<xml_diff>
--- a/Final 450/FINAL450.xlsx
+++ b/Final 450/FINAL450.xlsx
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C240" sqref="C240"/>
+    <sheetView tabSelected="1" topLeftCell="A251" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C263" sqref="C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4378,7 +4378,7 @@
         <v>233</v>
       </c>
       <c r="C240" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="241" spans="1:3" ht="21">
@@ -4466,7 +4466,7 @@
         <v>241</v>
       </c>
       <c r="C248" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="21">
@@ -4477,7 +4477,7 @@
         <v>242</v>
       </c>
       <c r="C249" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="250" spans="1:3" ht="21">
@@ -4576,7 +4576,7 @@
         <v>251</v>
       </c>
       <c r="C258" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="259" spans="1:3" ht="21">
@@ -4620,7 +4620,7 @@
         <v>255</v>
       </c>
       <c r="C262" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="263" spans="1:3" ht="21">
@@ -4631,7 +4631,7 @@
         <v>256</v>
       </c>
       <c r="C263" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="21">
@@ -5972,7 +5972,7 @@
         <v>377</v>
       </c>
       <c r="C390" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="391" spans="1:3" ht="21">
@@ -6593,7 +6593,7 @@
         <v>431</v>
       </c>
       <c r="C449" s="4" t="s">
-        <v>4</v>
+        <v>464</v>
       </c>
     </row>
     <row r="450" spans="1:3" ht="21">

</xml_diff>